<commit_message>
Add more treasure tables
</commit_message>
<xml_diff>
--- a/Individual Treasure Averages.xlsx
+++ b/Individual Treasure Averages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5937DBC2-7C6D-4910-9585-3D5ABE662A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72182FB-E997-4778-9D16-F612EC0E4FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="616" activeTab="1" xr2:uid="{5E3698F5-01A8-41EE-A738-BAB99CC962C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" tabRatio="616" activeTab="1" xr2:uid="{5E3698F5-01A8-41EE-A738-BAB99CC962C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Individual Treasure" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="86">
   <si>
     <t>Individual gp Per Formula</t>
   </si>
@@ -278,6 +281,24 @@
   </si>
   <si>
     <t>CR 13: Humanoid</t>
+  </si>
+  <si>
+    <t>CR 14 Individual Treasure Tables</t>
+  </si>
+  <si>
+    <t>CR 14: Humanoid</t>
+  </si>
+  <si>
+    <t>CR 15 Individual Treasure Tables</t>
+  </si>
+  <si>
+    <t>CR 15: Humanoid</t>
+  </si>
+  <si>
+    <t>CR 16 Individual Treasure Tables</t>
+  </si>
+  <si>
+    <t>CR 16: Humanoid</t>
   </si>
 </sst>
 </file>
@@ -656,9 +677,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -691,6 +709,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1637,10 +1658,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD8D082-213D-4692-B6C5-868C3C1BDB24}">
-  <dimension ref="A1:AD160"/>
+  <dimension ref="A1:AD190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="G124" sqref="G124"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="L178" sqref="L178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,20 +1700,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
       <c r="Z1" s="39"/>
       <c r="AA1" s="39"/>
       <c r="AB1" s="39"/>
@@ -1734,10 +1755,10 @@
       <c r="AD2" s="37"/>
     </row>
     <row r="3" spans="1:30" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="50"/>
+      <c r="B3" s="49"/>
       <c r="C3" s="21">
         <v>3</v>
       </c>
@@ -1932,18 +1953,18 @@
       </c>
     </row>
     <row r="10" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="55"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="33">
         <f>'Individual Treasure'!B3</f>
         <v>1.0794007754789445</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="57"/>
+      <c r="E10" s="56"/>
       <c r="F10" s="34">
         <f>SUMPRODUCT(C5:C9,F5:F9)</f>
         <v>1</v>
@@ -1969,20 +1990,20 @@
       <c r="AD10" s="13"/>
     </row>
     <row r="11" spans="1:30" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
       <c r="Z11" s="39"/>
       <c r="AA11" s="39"/>
       <c r="AB11" s="39"/>
@@ -1990,14 +2011,14 @@
       <c r="AD11" s="39"/>
     </row>
     <row r="12" spans="1:30" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="48"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="47"/>
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
       <c r="I12" s="37"/>
@@ -2024,18 +2045,18 @@
       <c r="AD12" s="37"/>
     </row>
     <row r="13" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="50"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="21">
         <v>3</v>
       </c>
-      <c r="D13" s="51" t="s">
+      <c r="D13" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="52"/>
-      <c r="F13" s="53"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="52"/>
       <c r="G13" s="38"/>
       <c r="H13" s="38"/>
       <c r="I13" s="36"/>
@@ -2192,18 +2213,18 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="55"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="33">
         <f>'Individual Treasure'!B4</f>
         <v>1.6717350674697367</v>
       </c>
-      <c r="D20" s="56" t="s">
+      <c r="D20" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="57"/>
+      <c r="E20" s="56"/>
       <c r="F20" s="34">
         <f>SUMPRODUCT(C15:C19,F15:F19)</f>
         <v>1.6750000000000003</v>
@@ -2212,64 +2233,64 @@
       <c r="K20" s="13"/>
     </row>
     <row r="21" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="46"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
     </row>
     <row r="22" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A22" s="47" t="s">
+      <c r="A22" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="47"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="47" t="s">
+      <c r="B22" s="46"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="47"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="48"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="47"/>
     </row>
     <row r="23" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="50"/>
+      <c r="B23" s="49"/>
       <c r="C23" s="21">
         <v>3</v>
       </c>
-      <c r="D23" s="51" t="s">
+      <c r="D23" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="52"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="49" t="s">
+      <c r="E23" s="51"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="H23" s="50"/>
+      <c r="H23" s="49"/>
       <c r="I23" s="21">
         <v>3</v>
       </c>
-      <c r="J23" s="51" t="s">
+      <c r="J23" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="K23" s="52"/>
-      <c r="L23" s="53"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="52"/>
     </row>
     <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="42" t="s">
@@ -2532,78 +2553,78 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="55"/>
+      <c r="B30" s="54"/>
       <c r="C30" s="33">
         <f>'Individual Treasure'!B5</f>
         <v>2.5891199999999999</v>
       </c>
-      <c r="D30" s="56" t="s">
+      <c r="D30" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="57"/>
+      <c r="E30" s="56"/>
       <c r="F30" s="34">
         <f>SUMPRODUCT(C25:C29,F25:F29)</f>
         <v>2.5750000000000002</v>
       </c>
-      <c r="G30" s="54" t="s">
+      <c r="G30" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="H30" s="55"/>
+      <c r="H30" s="54"/>
       <c r="I30" s="33">
         <f>'Individual Treasure'!B5</f>
         <v>2.5891199999999999</v>
       </c>
-      <c r="J30" s="56" t="s">
+      <c r="J30" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="K30" s="57"/>
+      <c r="K30" s="56"/>
       <c r="L30" s="34">
         <f>SUMPRODUCT(I25:I29,L25:L29)</f>
         <v>2.5499999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="57"/>
     </row>
     <row r="32" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="47"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="48"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="47"/>
     </row>
     <row r="33" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="50"/>
+      <c r="B33" s="49"/>
       <c r="C33" s="21">
         <v>3</v>
       </c>
-      <c r="D33" s="51" t="s">
+      <c r="D33" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E33" s="52"/>
-      <c r="F33" s="53"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="52"/>
     </row>
     <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="42" t="s">
@@ -2742,62 +2763,62 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="54" t="s">
+      <c r="A40" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="55"/>
+      <c r="B40" s="54"/>
       <c r="C40" s="33">
         <f>'Individual Treasure'!B6</f>
         <v>4.0099310619512103</v>
       </c>
-      <c r="D40" s="56" t="s">
+      <c r="D40" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="57"/>
+      <c r="E40" s="56"/>
       <c r="F40" s="34">
         <f>SUMPRODUCT(C35:C39,F35:F39)</f>
         <v>4.05</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="46"/>
-      <c r="C41" s="46"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="46"/>
-      <c r="H41" s="46"/>
-      <c r="I41" s="46"/>
-      <c r="J41" s="46"/>
-      <c r="K41" s="46"/>
-      <c r="L41" s="46"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="57"/>
+      <c r="J41" s="57"/>
+      <c r="K41" s="57"/>
+      <c r="L41" s="57"/>
     </row>
     <row r="42" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A42" s="47" t="s">
+      <c r="A42" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="47"/>
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="48"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="47"/>
     </row>
     <row r="43" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="50"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="21">
         <v>3</v>
       </c>
-      <c r="D43" s="51" t="s">
+      <c r="D43" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E43" s="52"/>
-      <c r="F43" s="53"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="52"/>
     </row>
     <row r="44" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="42" t="s">
@@ -2936,62 +2957,62 @@
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="54" t="s">
+      <c r="A50" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="55"/>
+      <c r="B50" s="54"/>
       <c r="C50" s="33">
         <f>'Individual Treasure'!B7</f>
         <v>6.2104294592761873</v>
       </c>
-      <c r="D50" s="56" t="s">
+      <c r="D50" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E50" s="57"/>
+      <c r="E50" s="56"/>
       <c r="F50" s="34">
         <f>SUMPRODUCT(C45:C49,F45:F49)</f>
         <v>6.2000000000000011</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="46" t="s">
+      <c r="A51" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="46"/>
-      <c r="C51" s="46"/>
-      <c r="D51" s="46"/>
-      <c r="E51" s="46"/>
-      <c r="F51" s="46"/>
-      <c r="G51" s="46"/>
-      <c r="H51" s="46"/>
-      <c r="I51" s="46"/>
-      <c r="J51" s="46"/>
-      <c r="K51" s="46"/>
-      <c r="L51" s="46"/>
+      <c r="B51" s="57"/>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
+      <c r="H51" s="57"/>
+      <c r="I51" s="57"/>
+      <c r="J51" s="57"/>
+      <c r="K51" s="57"/>
+      <c r="L51" s="57"/>
     </row>
     <row r="52" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A52" s="47" t="s">
+      <c r="A52" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="B52" s="47"/>
-      <c r="C52" s="47"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="48"/>
+      <c r="B52" s="46"/>
+      <c r="C52" s="46"/>
+      <c r="D52" s="46"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="47"/>
     </row>
     <row r="53" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="49" t="s">
+      <c r="A53" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B53" s="50"/>
+      <c r="B53" s="49"/>
       <c r="C53" s="21">
         <v>3</v>
       </c>
-      <c r="D53" s="51" t="s">
+      <c r="D53" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E53" s="52"/>
-      <c r="F53" s="53"/>
+      <c r="E53" s="51"/>
+      <c r="F53" s="52"/>
     </row>
     <row r="54" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="42" t="s">
@@ -3130,62 +3151,62 @@
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="54" t="s">
+      <c r="A60" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B60" s="55"/>
+      <c r="B60" s="54"/>
       <c r="C60" s="33">
         <f>'Individual Treasure'!B8</f>
         <v>9.6184780917100969</v>
       </c>
-      <c r="D60" s="56" t="s">
+      <c r="D60" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E60" s="57"/>
+      <c r="E60" s="56"/>
       <c r="F60" s="34">
         <f>SUMPRODUCT(C55:C59,F55:F59)</f>
         <v>9.6000000000000014</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="46" t="s">
+      <c r="A61" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="46"/>
-      <c r="C61" s="46"/>
-      <c r="D61" s="46"/>
-      <c r="E61" s="46"/>
-      <c r="F61" s="46"/>
-      <c r="G61" s="46"/>
-      <c r="H61" s="46"/>
-      <c r="I61" s="46"/>
-      <c r="J61" s="46"/>
-      <c r="K61" s="46"/>
-      <c r="L61" s="46"/>
+      <c r="B61" s="57"/>
+      <c r="C61" s="57"/>
+      <c r="D61" s="57"/>
+      <c r="E61" s="57"/>
+      <c r="F61" s="57"/>
+      <c r="G61" s="57"/>
+      <c r="H61" s="57"/>
+      <c r="I61" s="57"/>
+      <c r="J61" s="57"/>
+      <c r="K61" s="57"/>
+      <c r="L61" s="57"/>
     </row>
     <row r="62" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A62" s="47" t="s">
+      <c r="A62" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="B62" s="47"/>
-      <c r="C62" s="47"/>
-      <c r="D62" s="47"/>
-      <c r="E62" s="47"/>
-      <c r="F62" s="48"/>
+      <c r="B62" s="46"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="46"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="47"/>
     </row>
     <row r="63" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="49" t="s">
+      <c r="A63" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B63" s="50"/>
+      <c r="B63" s="49"/>
       <c r="C63" s="21">
         <v>3</v>
       </c>
-      <c r="D63" s="51" t="s">
+      <c r="D63" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E63" s="52"/>
-      <c r="F63" s="53"/>
+      <c r="E63" s="51"/>
+      <c r="F63" s="52"/>
     </row>
     <row r="64" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="42" t="s">
@@ -3324,62 +3345,62 @@
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="54" t="s">
+      <c r="A70" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B70" s="55"/>
+      <c r="B70" s="54"/>
       <c r="C70" s="33">
         <f>'Individual Treasure'!B9</f>
         <v>14.89673482443669</v>
       </c>
-      <c r="D70" s="56" t="s">
+      <c r="D70" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E70" s="57"/>
+      <c r="E70" s="56"/>
       <c r="F70" s="34">
         <f>SUMPRODUCT(C65:C69,F65:F69)</f>
         <v>14.900000000000002</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="46" t="s">
+      <c r="A71" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="B71" s="46"/>
-      <c r="C71" s="46"/>
-      <c r="D71" s="46"/>
-      <c r="E71" s="46"/>
-      <c r="F71" s="46"/>
-      <c r="G71" s="46"/>
-      <c r="H71" s="46"/>
-      <c r="I71" s="46"/>
-      <c r="J71" s="46"/>
-      <c r="K71" s="46"/>
-      <c r="L71" s="46"/>
+      <c r="B71" s="57"/>
+      <c r="C71" s="57"/>
+      <c r="D71" s="57"/>
+      <c r="E71" s="57"/>
+      <c r="F71" s="57"/>
+      <c r="G71" s="57"/>
+      <c r="H71" s="57"/>
+      <c r="I71" s="57"/>
+      <c r="J71" s="57"/>
+      <c r="K71" s="57"/>
+      <c r="L71" s="57"/>
     </row>
     <row r="72" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A72" s="47" t="s">
+      <c r="A72" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="B72" s="47"/>
-      <c r="C72" s="47"/>
-      <c r="D72" s="47"/>
-      <c r="E72" s="47"/>
-      <c r="F72" s="48"/>
+      <c r="B72" s="46"/>
+      <c r="C72" s="46"/>
+      <c r="D72" s="46"/>
+      <c r="E72" s="46"/>
+      <c r="F72" s="47"/>
     </row>
     <row r="73" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="49" t="s">
+      <c r="A73" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B73" s="50"/>
+      <c r="B73" s="49"/>
       <c r="C73" s="21">
         <v>5</v>
       </c>
-      <c r="D73" s="51" t="s">
+      <c r="D73" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E73" s="52"/>
-      <c r="F73" s="53"/>
+      <c r="E73" s="51"/>
+      <c r="F73" s="52"/>
     </row>
     <row r="74" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="42" t="s">
@@ -3518,62 +3539,62 @@
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" s="54" t="s">
+      <c r="A80" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B80" s="55"/>
+      <c r="B80" s="54"/>
       <c r="C80" s="33">
         <f>'Individual Treasure'!B10</f>
         <v>23.071499078512772</v>
       </c>
-      <c r="D80" s="56" t="s">
+      <c r="D80" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E80" s="57"/>
+      <c r="E80" s="56"/>
       <c r="F80" s="34">
         <f>SUMPRODUCT(C75:C79,F75:F79)</f>
         <v>23</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="46" t="s">
+      <c r="A81" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="B81" s="46"/>
-      <c r="C81" s="46"/>
-      <c r="D81" s="46"/>
-      <c r="E81" s="46"/>
-      <c r="F81" s="46"/>
-      <c r="G81" s="46"/>
-      <c r="H81" s="46"/>
-      <c r="I81" s="46"/>
-      <c r="J81" s="46"/>
-      <c r="K81" s="46"/>
-      <c r="L81" s="46"/>
+      <c r="B81" s="57"/>
+      <c r="C81" s="57"/>
+      <c r="D81" s="57"/>
+      <c r="E81" s="57"/>
+      <c r="F81" s="57"/>
+      <c r="G81" s="57"/>
+      <c r="H81" s="57"/>
+      <c r="I81" s="57"/>
+      <c r="J81" s="57"/>
+      <c r="K81" s="57"/>
+      <c r="L81" s="57"/>
     </row>
     <row r="82" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A82" s="47" t="s">
+      <c r="A82" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="B82" s="47"/>
-      <c r="C82" s="47"/>
-      <c r="D82" s="47"/>
-      <c r="E82" s="47"/>
-      <c r="F82" s="48"/>
+      <c r="B82" s="46"/>
+      <c r="C82" s="46"/>
+      <c r="D82" s="46"/>
+      <c r="E82" s="46"/>
+      <c r="F82" s="47"/>
     </row>
     <row r="83" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="49" t="s">
+      <c r="A83" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B83" s="50"/>
+      <c r="B83" s="49"/>
       <c r="C83" s="21">
         <v>5</v>
       </c>
-      <c r="D83" s="51" t="s">
+      <c r="D83" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E83" s="52"/>
-      <c r="F83" s="53"/>
+      <c r="E83" s="51"/>
+      <c r="F83" s="52"/>
     </row>
     <row r="84" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="42" t="s">
@@ -3712,62 +3733,62 @@
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A90" s="54" t="s">
+      <c r="A90" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B90" s="55"/>
+      <c r="B90" s="54"/>
       <c r="C90" s="33">
         <f>'Individual Treasure'!B11</f>
         <v>35.732264553480377</v>
       </c>
-      <c r="D90" s="56" t="s">
+      <c r="D90" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E90" s="57"/>
+      <c r="E90" s="56"/>
       <c r="F90" s="34">
         <f>SUMPRODUCT(C85:C89,F85:F89)</f>
         <v>35</v>
       </c>
     </row>
     <row r="91" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="46" t="s">
+      <c r="A91" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="B91" s="46"/>
-      <c r="C91" s="46"/>
-      <c r="D91" s="46"/>
-      <c r="E91" s="46"/>
-      <c r="F91" s="46"/>
-      <c r="G91" s="46"/>
-      <c r="H91" s="46"/>
-      <c r="I91" s="46"/>
-      <c r="J91" s="46"/>
-      <c r="K91" s="46"/>
-      <c r="L91" s="46"/>
+      <c r="B91" s="57"/>
+      <c r="C91" s="57"/>
+      <c r="D91" s="57"/>
+      <c r="E91" s="57"/>
+      <c r="F91" s="57"/>
+      <c r="G91" s="57"/>
+      <c r="H91" s="57"/>
+      <c r="I91" s="57"/>
+      <c r="J91" s="57"/>
+      <c r="K91" s="57"/>
+      <c r="L91" s="57"/>
     </row>
     <row r="92" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A92" s="47" t="s">
+      <c r="A92" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="B92" s="47"/>
-      <c r="C92" s="47"/>
-      <c r="D92" s="47"/>
-      <c r="E92" s="47"/>
-      <c r="F92" s="48"/>
+      <c r="B92" s="46"/>
+      <c r="C92" s="46"/>
+      <c r="D92" s="46"/>
+      <c r="E92" s="46"/>
+      <c r="F92" s="47"/>
     </row>
     <row r="93" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="49" t="s">
+      <c r="A93" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B93" s="50"/>
+      <c r="B93" s="49"/>
       <c r="C93" s="21">
         <v>5</v>
       </c>
-      <c r="D93" s="51" t="s">
+      <c r="D93" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E93" s="52"/>
-      <c r="F93" s="53"/>
+      <c r="E93" s="51"/>
+      <c r="F93" s="52"/>
     </row>
     <row r="94" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="42" t="s">
@@ -3906,62 +3927,62 @@
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A100" s="54" t="s">
+      <c r="A100" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B100" s="55"/>
+      <c r="B100" s="54"/>
       <c r="C100" s="33">
         <f>'Individual Treasure'!B12</f>
         <v>55.340778931397217</v>
       </c>
-      <c r="D100" s="56" t="s">
+      <c r="D100" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E100" s="57"/>
+      <c r="E100" s="56"/>
       <c r="F100" s="34">
         <f>SUMPRODUCT(C95:C99,F95:F99)</f>
         <v>55.25</v>
       </c>
     </row>
     <row r="101" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A101" s="46" t="s">
+      <c r="A101" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="B101" s="46"/>
-      <c r="C101" s="46"/>
-      <c r="D101" s="46"/>
-      <c r="E101" s="46"/>
-      <c r="F101" s="46"/>
-      <c r="G101" s="46"/>
-      <c r="H101" s="46"/>
-      <c r="I101" s="46"/>
-      <c r="J101" s="46"/>
-      <c r="K101" s="46"/>
-      <c r="L101" s="46"/>
+      <c r="B101" s="57"/>
+      <c r="C101" s="57"/>
+      <c r="D101" s="57"/>
+      <c r="E101" s="57"/>
+      <c r="F101" s="57"/>
+      <c r="G101" s="57"/>
+      <c r="H101" s="57"/>
+      <c r="I101" s="57"/>
+      <c r="J101" s="57"/>
+      <c r="K101" s="57"/>
+      <c r="L101" s="57"/>
     </row>
     <row r="102" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A102" s="47" t="s">
+      <c r="A102" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="B102" s="47"/>
-      <c r="C102" s="47"/>
-      <c r="D102" s="47"/>
-      <c r="E102" s="47"/>
-      <c r="F102" s="48"/>
+      <c r="B102" s="46"/>
+      <c r="C102" s="46"/>
+      <c r="D102" s="46"/>
+      <c r="E102" s="46"/>
+      <c r="F102" s="47"/>
     </row>
     <row r="103" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="49" t="s">
+      <c r="A103" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B103" s="50"/>
+      <c r="B103" s="49"/>
       <c r="C103" s="21">
         <v>5</v>
       </c>
-      <c r="D103" s="51" t="s">
+      <c r="D103" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E103" s="52"/>
-      <c r="F103" s="53"/>
+      <c r="E103" s="51"/>
+      <c r="F103" s="52"/>
     </row>
     <row r="104" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="42" t="s">
@@ -4100,62 +4121,62 @@
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A110" s="54" t="s">
+      <c r="A110" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B110" s="55"/>
+      <c r="B110" s="54"/>
       <c r="C110" s="33">
         <f>'Individual Treasure'!B13</f>
         <v>85.709703849023938</v>
       </c>
-      <c r="D110" s="56" t="s">
+      <c r="D110" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E110" s="57"/>
+      <c r="E110" s="56"/>
       <c r="F110" s="34">
         <f>SUMPRODUCT(C105:C109,F105:F109)</f>
         <v>85.5</v>
       </c>
     </row>
     <row r="111" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A111" s="46" t="s">
+      <c r="A111" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="B111" s="46"/>
-      <c r="C111" s="46"/>
-      <c r="D111" s="46"/>
-      <c r="E111" s="46"/>
-      <c r="F111" s="46"/>
-      <c r="G111" s="46"/>
-      <c r="H111" s="46"/>
-      <c r="I111" s="46"/>
-      <c r="J111" s="46"/>
-      <c r="K111" s="46"/>
-      <c r="L111" s="46"/>
+      <c r="B111" s="57"/>
+      <c r="C111" s="57"/>
+      <c r="D111" s="57"/>
+      <c r="E111" s="57"/>
+      <c r="F111" s="57"/>
+      <c r="G111" s="57"/>
+      <c r="H111" s="57"/>
+      <c r="I111" s="57"/>
+      <c r="J111" s="57"/>
+      <c r="K111" s="57"/>
+      <c r="L111" s="57"/>
     </row>
     <row r="112" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A112" s="47" t="s">
+      <c r="A112" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="B112" s="47"/>
-      <c r="C112" s="47"/>
-      <c r="D112" s="47"/>
-      <c r="E112" s="47"/>
-      <c r="F112" s="48"/>
+      <c r="B112" s="46"/>
+      <c r="C112" s="46"/>
+      <c r="D112" s="46"/>
+      <c r="E112" s="46"/>
+      <c r="F112" s="47"/>
     </row>
     <row r="113" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="49" t="s">
+      <c r="A113" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B113" s="50"/>
+      <c r="B113" s="49"/>
       <c r="C113" s="21">
         <v>5</v>
       </c>
-      <c r="D113" s="51" t="s">
+      <c r="D113" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E113" s="52"/>
-      <c r="F113" s="53"/>
+      <c r="E113" s="51"/>
+      <c r="F113" s="52"/>
     </row>
     <row r="114" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="42" t="s">
@@ -4294,62 +4315,62 @@
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A120" s="54" t="s">
+      <c r="A120" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B120" s="55"/>
+      <c r="B120" s="54"/>
       <c r="C120" s="33">
         <f>'Individual Treasure'!B14</f>
         <v>132.7439453462336</v>
       </c>
-      <c r="D120" s="56" t="s">
+      <c r="D120" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E120" s="57"/>
+      <c r="E120" s="56"/>
       <c r="F120" s="34">
         <f>SUMPRODUCT(C115:C119,F115:F119)</f>
         <v>133</v>
       </c>
     </row>
     <row r="121" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A121" s="46" t="s">
+      <c r="A121" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="B121" s="46"/>
-      <c r="C121" s="46"/>
-      <c r="D121" s="46"/>
-      <c r="E121" s="46"/>
-      <c r="F121" s="46"/>
-      <c r="G121" s="46"/>
-      <c r="H121" s="46"/>
-      <c r="I121" s="46"/>
-      <c r="J121" s="46"/>
-      <c r="K121" s="46"/>
-      <c r="L121" s="46"/>
+      <c r="B121" s="57"/>
+      <c r="C121" s="57"/>
+      <c r="D121" s="57"/>
+      <c r="E121" s="57"/>
+      <c r="F121" s="57"/>
+      <c r="G121" s="57"/>
+      <c r="H121" s="57"/>
+      <c r="I121" s="57"/>
+      <c r="J121" s="57"/>
+      <c r="K121" s="57"/>
+      <c r="L121" s="57"/>
     </row>
     <row r="122" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A122" s="47" t="s">
+      <c r="A122" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="B122" s="47"/>
-      <c r="C122" s="47"/>
-      <c r="D122" s="47"/>
-      <c r="E122" s="47"/>
-      <c r="F122" s="48"/>
+      <c r="B122" s="46"/>
+      <c r="C122" s="46"/>
+      <c r="D122" s="46"/>
+      <c r="E122" s="46"/>
+      <c r="F122" s="47"/>
     </row>
     <row r="123" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A123" s="49" t="s">
+      <c r="A123" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B123" s="50"/>
+      <c r="B123" s="49"/>
       <c r="C123" s="21">
         <v>5</v>
       </c>
-      <c r="D123" s="51" t="s">
+      <c r="D123" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E123" s="52"/>
-      <c r="F123" s="53"/>
+      <c r="E123" s="51"/>
+      <c r="F123" s="52"/>
     </row>
     <row r="124" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="42" t="s">
@@ -4488,62 +4509,62 @@
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A130" s="54" t="s">
+      <c r="A130" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B130" s="55"/>
+      <c r="B130" s="54"/>
       <c r="C130" s="33">
         <f>'Individual Treasure'!B15</f>
         <v>205.58879840633722</v>
       </c>
-      <c r="D130" s="56" t="s">
+      <c r="D130" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E130" s="57"/>
+      <c r="E130" s="56"/>
       <c r="F130" s="34">
         <f>SUMPRODUCT(C125:C129,F125:F129)</f>
         <v>205</v>
       </c>
     </row>
     <row r="131" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A131" s="46" t="s">
+      <c r="A131" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="B131" s="46"/>
-      <c r="C131" s="46"/>
-      <c r="D131" s="46"/>
-      <c r="E131" s="46"/>
-      <c r="F131" s="46"/>
-      <c r="G131" s="46"/>
-      <c r="H131" s="46"/>
-      <c r="I131" s="46"/>
-      <c r="J131" s="46"/>
-      <c r="K131" s="46"/>
-      <c r="L131" s="46"/>
+      <c r="B131" s="57"/>
+      <c r="C131" s="57"/>
+      <c r="D131" s="57"/>
+      <c r="E131" s="57"/>
+      <c r="F131" s="57"/>
+      <c r="G131" s="57"/>
+      <c r="H131" s="57"/>
+      <c r="I131" s="57"/>
+      <c r="J131" s="57"/>
+      <c r="K131" s="57"/>
+      <c r="L131" s="57"/>
     </row>
     <row r="132" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A132" s="47" t="s">
+      <c r="A132" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="B132" s="47"/>
-      <c r="C132" s="47"/>
-      <c r="D132" s="47"/>
-      <c r="E132" s="47"/>
-      <c r="F132" s="48"/>
+      <c r="B132" s="46"/>
+      <c r="C132" s="46"/>
+      <c r="D132" s="46"/>
+      <c r="E132" s="46"/>
+      <c r="F132" s="47"/>
     </row>
     <row r="133" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A133" s="49" t="s">
+      <c r="A133" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B133" s="50"/>
+      <c r="B133" s="49"/>
       <c r="C133" s="21">
         <v>7</v>
       </c>
-      <c r="D133" s="51" t="s">
+      <c r="D133" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E133" s="52"/>
-      <c r="F133" s="53"/>
+      <c r="E133" s="51"/>
+      <c r="F133" s="52"/>
     </row>
     <row r="134" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="42" t="s">
@@ -4682,62 +4703,62 @@
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A140" s="54" t="s">
+      <c r="A140" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B140" s="55"/>
+      <c r="B140" s="54"/>
       <c r="C140" s="33">
         <f>'Individual Treasure'!B16</f>
         <v>318.40814976470659</v>
       </c>
-      <c r="D140" s="56" t="s">
+      <c r="D140" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E140" s="57"/>
+      <c r="E140" s="56"/>
       <c r="F140" s="34">
         <f>SUMPRODUCT(C135:C139,F135:F139)</f>
         <v>317.5</v>
       </c>
     </row>
     <row r="141" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A141" s="46" t="s">
+      <c r="A141" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="B141" s="46"/>
-      <c r="C141" s="46"/>
-      <c r="D141" s="46"/>
-      <c r="E141" s="46"/>
-      <c r="F141" s="46"/>
-      <c r="G141" s="46"/>
-      <c r="H141" s="46"/>
-      <c r="I141" s="46"/>
-      <c r="J141" s="46"/>
-      <c r="K141" s="46"/>
-      <c r="L141" s="46"/>
+      <c r="B141" s="57"/>
+      <c r="C141" s="57"/>
+      <c r="D141" s="57"/>
+      <c r="E141" s="57"/>
+      <c r="F141" s="57"/>
+      <c r="G141" s="57"/>
+      <c r="H141" s="57"/>
+      <c r="I141" s="57"/>
+      <c r="J141" s="57"/>
+      <c r="K141" s="57"/>
+      <c r="L141" s="57"/>
     </row>
     <row r="142" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A142" s="47" t="s">
+      <c r="A142" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="B142" s="47"/>
-      <c r="C142" s="47"/>
-      <c r="D142" s="47"/>
-      <c r="E142" s="47"/>
-      <c r="F142" s="48"/>
+      <c r="B142" s="46"/>
+      <c r="C142" s="46"/>
+      <c r="D142" s="46"/>
+      <c r="E142" s="46"/>
+      <c r="F142" s="47"/>
     </row>
     <row r="143" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A143" s="49" t="s">
+      <c r="A143" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B143" s="50"/>
+      <c r="B143" s="49"/>
       <c r="C143" s="21">
         <v>7</v>
       </c>
-      <c r="D143" s="51" t="s">
+      <c r="D143" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E143" s="52"/>
-      <c r="F143" s="53"/>
+      <c r="E143" s="51"/>
+      <c r="F143" s="52"/>
     </row>
     <row r="144" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="42" t="s">
@@ -4876,62 +4897,62 @@
       </c>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A150" s="54" t="s">
+      <c r="A150" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B150" s="55"/>
+      <c r="B150" s="54"/>
       <c r="C150" s="33">
         <f>'Individual Treasure'!B17</f>
         <v>493.13849111663814</v>
       </c>
-      <c r="D150" s="56" t="s">
+      <c r="D150" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E150" s="57"/>
+      <c r="E150" s="56"/>
       <c r="F150" s="34">
         <f>SUMPRODUCT(C145:C149,F145:F149)</f>
         <v>495</v>
       </c>
     </row>
     <row r="151" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A151" s="46" t="s">
+      <c r="A151" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="B151" s="46"/>
-      <c r="C151" s="46"/>
-      <c r="D151" s="46"/>
-      <c r="E151" s="46"/>
-      <c r="F151" s="46"/>
-      <c r="G151" s="46"/>
-      <c r="H151" s="46"/>
-      <c r="I151" s="46"/>
-      <c r="J151" s="46"/>
-      <c r="K151" s="46"/>
-      <c r="L151" s="46"/>
+      <c r="B151" s="57"/>
+      <c r="C151" s="57"/>
+      <c r="D151" s="57"/>
+      <c r="E151" s="57"/>
+      <c r="F151" s="57"/>
+      <c r="G151" s="57"/>
+      <c r="H151" s="57"/>
+      <c r="I151" s="57"/>
+      <c r="J151" s="57"/>
+      <c r="K151" s="57"/>
+      <c r="L151" s="57"/>
     </row>
     <row r="152" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A152" s="47" t="s">
+      <c r="A152" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="B152" s="47"/>
-      <c r="C152" s="47"/>
-      <c r="D152" s="47"/>
-      <c r="E152" s="47"/>
-      <c r="F152" s="48"/>
+      <c r="B152" s="46"/>
+      <c r="C152" s="46"/>
+      <c r="D152" s="46"/>
+      <c r="E152" s="46"/>
+      <c r="F152" s="47"/>
     </row>
     <row r="153" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A153" s="49" t="s">
+      <c r="A153" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B153" s="50"/>
+      <c r="B153" s="49"/>
       <c r="C153" s="21">
         <v>7</v>
       </c>
-      <c r="D153" s="51" t="s">
+      <c r="D153" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E153" s="52"/>
-      <c r="F153" s="53"/>
+      <c r="E153" s="51"/>
+      <c r="F153" s="52"/>
     </row>
     <row r="154" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="42" t="s">
@@ -5070,34 +5091,697 @@
       </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A160" s="54" t="s">
+      <c r="A160" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B160" s="55"/>
+      <c r="B160" s="54"/>
       <c r="C160" s="33">
         <f>'Individual Treasure'!B18</f>
         <v>763.75423053869986</v>
       </c>
-      <c r="D160" s="56" t="s">
+      <c r="D160" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E160" s="57"/>
+      <c r="E160" s="56"/>
       <c r="F160" s="34">
         <f>SUMPRODUCT(C155:C159,F155:F159)</f>
         <v>760</v>
       </c>
     </row>
+    <row r="161" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A161" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="B161" s="57"/>
+      <c r="C161" s="57"/>
+      <c r="D161" s="57"/>
+      <c r="E161" s="57"/>
+      <c r="F161" s="57"/>
+      <c r="G161" s="57"/>
+      <c r="H161" s="57"/>
+      <c r="I161" s="57"/>
+      <c r="J161" s="57"/>
+      <c r="K161" s="57"/>
+      <c r="L161" s="57"/>
+    </row>
+    <row r="162" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A162" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="B162" s="46"/>
+      <c r="C162" s="46"/>
+      <c r="D162" s="46"/>
+      <c r="E162" s="46"/>
+      <c r="F162" s="47"/>
+    </row>
+    <row r="163" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A163" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B163" s="49"/>
+      <c r="C163" s="21">
+        <v>7</v>
+      </c>
+      <c r="D163" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="E163" s="51"/>
+      <c r="F163" s="52"/>
+    </row>
+    <row r="164" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A164" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B164" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C164" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D164" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E164" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F164" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A165" s="43">
+        <f>C163+1</f>
+        <v>8</v>
+      </c>
+      <c r="B165" s="8">
+        <v>9</v>
+      </c>
+      <c r="C165" s="31">
+        <f>((B165-A165+1)*0.05)</f>
+        <v>0.1</v>
+      </c>
+      <c r="D165" s="18">
+        <v>3</v>
+      </c>
+      <c r="E165" s="8">
+        <v>100</v>
+      </c>
+      <c r="F165" s="19">
+        <f>D165*E165</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A166" s="43">
+        <f>B165+1</f>
+        <v>10</v>
+      </c>
+      <c r="B166" s="8">
+        <v>14</v>
+      </c>
+      <c r="C166" s="31">
+        <f t="shared" ref="C166:C169" si="51">((B166-A166+1)*0.05)</f>
+        <v>0.25</v>
+      </c>
+      <c r="D166" s="18">
+        <v>1</v>
+      </c>
+      <c r="E166" s="8">
+        <v>500</v>
+      </c>
+      <c r="F166" s="19">
+        <f t="shared" ref="F166:F169" si="52">D166*E166</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A167" s="43">
+        <f t="shared" ref="A167:A169" si="53">B166+1</f>
+        <v>15</v>
+      </c>
+      <c r="B167" s="8">
+        <v>20</v>
+      </c>
+      <c r="C167" s="31">
+        <f t="shared" si="51"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="D167" s="18">
+        <v>2</v>
+      </c>
+      <c r="E167" s="8">
+        <v>500</v>
+      </c>
+      <c r="F167" s="19">
+        <f t="shared" si="52"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A168" s="43">
+        <f t="shared" si="53"/>
+        <v>21</v>
+      </c>
+      <c r="B168" s="8">
+        <v>26</v>
+      </c>
+      <c r="C168" s="31">
+        <f t="shared" si="51"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="D168" s="18">
+        <v>2</v>
+      </c>
+      <c r="E168" s="8">
+        <v>1000</v>
+      </c>
+      <c r="F168" s="19">
+        <f t="shared" si="52"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A169" s="43">
+        <f t="shared" si="53"/>
+        <v>27</v>
+      </c>
+      <c r="B169" s="44">
+        <f>20+C163</f>
+        <v>27</v>
+      </c>
+      <c r="C169" s="31">
+        <f t="shared" si="51"/>
+        <v>0.05</v>
+      </c>
+      <c r="D169" s="20">
+        <v>3</v>
+      </c>
+      <c r="E169" s="28">
+        <v>1000</v>
+      </c>
+      <c r="F169" s="22">
+        <f t="shared" si="52"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A170" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B170" s="54"/>
+      <c r="C170" s="33">
+        <f>'Individual Treasure'!B19</f>
+        <v>1182.8736453829017</v>
+      </c>
+      <c r="D170" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="E170" s="56"/>
+      <c r="F170" s="34">
+        <f>SUMPRODUCT(C165:C169,F165:F169)</f>
+        <v>1205.0000000000002</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A171" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="B171" s="57"/>
+      <c r="C171" s="57"/>
+      <c r="D171" s="57"/>
+      <c r="E171" s="57"/>
+      <c r="F171" s="57"/>
+      <c r="G171" s="57"/>
+      <c r="H171" s="57"/>
+      <c r="I171" s="57"/>
+      <c r="J171" s="57"/>
+      <c r="K171" s="57"/>
+      <c r="L171" s="57"/>
+    </row>
+    <row r="172" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A172" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B172" s="46"/>
+      <c r="C172" s="46"/>
+      <c r="D172" s="46"/>
+      <c r="E172" s="46"/>
+      <c r="F172" s="47"/>
+    </row>
+    <row r="173" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A173" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B173" s="49"/>
+      <c r="C173" s="21">
+        <v>7</v>
+      </c>
+      <c r="D173" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="E173" s="51"/>
+      <c r="F173" s="52"/>
+    </row>
+    <row r="174" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A174" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B174" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C174" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D174" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E174" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F174" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A175" s="43">
+        <f>C173+1</f>
+        <v>8</v>
+      </c>
+      <c r="B175" s="8">
+        <v>9</v>
+      </c>
+      <c r="C175" s="31">
+        <f>((B175-A175+1)*0.05)</f>
+        <v>0.1</v>
+      </c>
+      <c r="D175" s="18">
+        <v>1</v>
+      </c>
+      <c r="E175" s="8">
+        <v>500</v>
+      </c>
+      <c r="F175" s="19">
+        <f>D175*E175</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A176" s="43">
+        <f>B175+1</f>
+        <v>10</v>
+      </c>
+      <c r="B176" s="8">
+        <v>12</v>
+      </c>
+      <c r="C176" s="31">
+        <f t="shared" ref="C176:C179" si="54">((B176-A176+1)*0.05)</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="D176" s="18">
+        <v>2</v>
+      </c>
+      <c r="E176" s="8">
+        <v>500</v>
+      </c>
+      <c r="F176" s="19">
+        <f t="shared" ref="F176:F179" si="55">D176*E176</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A177" s="43">
+        <f t="shared" ref="A177:A179" si="56">B176+1</f>
+        <v>13</v>
+      </c>
+      <c r="B177" s="8">
+        <v>18</v>
+      </c>
+      <c r="C177" s="31">
+        <f t="shared" si="54"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="D177" s="18">
+        <v>3</v>
+      </c>
+      <c r="E177" s="8">
+        <v>500</v>
+      </c>
+      <c r="F177" s="19">
+        <f t="shared" si="55"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A178" s="43">
+        <f t="shared" si="56"/>
+        <v>19</v>
+      </c>
+      <c r="B178" s="8">
+        <v>24</v>
+      </c>
+      <c r="C178" s="31">
+        <f t="shared" si="54"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="D178" s="18">
+        <v>2</v>
+      </c>
+      <c r="E178" s="8">
+        <v>1000</v>
+      </c>
+      <c r="F178" s="19">
+        <f t="shared" si="55"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A179" s="43">
+        <f t="shared" si="56"/>
+        <v>25</v>
+      </c>
+      <c r="B179" s="44">
+        <f>20+C173</f>
+        <v>27</v>
+      </c>
+      <c r="C179" s="31">
+        <f t="shared" si="54"/>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="D179" s="20">
+        <v>2</v>
+      </c>
+      <c r="E179" s="28">
+        <v>2000</v>
+      </c>
+      <c r="F179" s="22">
+        <f t="shared" si="55"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A180" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B180" s="54"/>
+      <c r="C180" s="33">
+        <f>'Individual Treasure'!B20</f>
+        <v>1831.989932094441</v>
+      </c>
+      <c r="D180" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="E180" s="56"/>
+      <c r="F180" s="34">
+        <f>SUMPRODUCT(C175:C179,F175:F179)</f>
+        <v>1850.0000000000005</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A181" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="B181" s="57"/>
+      <c r="C181" s="57"/>
+      <c r="D181" s="57"/>
+      <c r="E181" s="57"/>
+      <c r="F181" s="57"/>
+      <c r="G181" s="57"/>
+      <c r="H181" s="57"/>
+      <c r="I181" s="57"/>
+      <c r="J181" s="57"/>
+      <c r="K181" s="57"/>
+      <c r="L181" s="57"/>
+    </row>
+    <row r="182" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A182" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B182" s="46"/>
+      <c r="C182" s="46"/>
+      <c r="D182" s="46"/>
+      <c r="E182" s="46"/>
+      <c r="F182" s="47"/>
+    </row>
+    <row r="183" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A183" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B183" s="49"/>
+      <c r="C183" s="21">
+        <v>7</v>
+      </c>
+      <c r="D183" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="E183" s="51"/>
+      <c r="F183" s="52"/>
+    </row>
+    <row r="184" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A184" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B184" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C184" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D184" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E184" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F184" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A185" s="43">
+        <f>C183+1</f>
+        <v>8</v>
+      </c>
+      <c r="B185" s="8">
+        <v>9</v>
+      </c>
+      <c r="C185" s="31">
+        <f>((B185-A185+1)*0.05)</f>
+        <v>0.1</v>
+      </c>
+      <c r="D185" s="18">
+        <v>1</v>
+      </c>
+      <c r="E185" s="8">
+        <v>500</v>
+      </c>
+      <c r="F185" s="19">
+        <f>D185*E185</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A186" s="43">
+        <f>B185+1</f>
+        <v>10</v>
+      </c>
+      <c r="B186" s="8">
+        <v>11</v>
+      </c>
+      <c r="C186" s="31">
+        <f t="shared" ref="C186:C189" si="57">((B186-A186+1)*0.05)</f>
+        <v>0.1</v>
+      </c>
+      <c r="D186" s="18">
+        <v>1</v>
+      </c>
+      <c r="E186" s="8">
+        <v>1000</v>
+      </c>
+      <c r="F186" s="19">
+        <f t="shared" ref="F186:F189" si="58">D186*E186</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A187" s="43">
+        <f t="shared" ref="A187:A189" si="59">B186+1</f>
+        <v>12</v>
+      </c>
+      <c r="B187" s="8">
+        <v>17</v>
+      </c>
+      <c r="C187" s="31">
+        <f t="shared" si="57"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="D187" s="18">
+        <v>2</v>
+      </c>
+      <c r="E187" s="8">
+        <v>1000</v>
+      </c>
+      <c r="F187" s="19">
+        <f t="shared" si="58"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A188" s="43">
+        <f t="shared" si="59"/>
+        <v>18</v>
+      </c>
+      <c r="B188" s="8">
+        <v>23</v>
+      </c>
+      <c r="C188" s="31">
+        <f t="shared" si="57"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="D188" s="18">
+        <v>3</v>
+      </c>
+      <c r="E188" s="8">
+        <v>1000</v>
+      </c>
+      <c r="F188" s="19">
+        <f t="shared" si="58"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A189" s="43">
+        <f t="shared" si="59"/>
+        <v>24</v>
+      </c>
+      <c r="B189" s="44">
+        <f>20+C183</f>
+        <v>27</v>
+      </c>
+      <c r="C189" s="31">
+        <f t="shared" si="57"/>
+        <v>0.2</v>
+      </c>
+      <c r="D189" s="20">
+        <v>3</v>
+      </c>
+      <c r="E189" s="28">
+        <v>2000</v>
+      </c>
+      <c r="F189" s="22">
+        <f t="shared" si="58"/>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A190" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B190" s="54"/>
+      <c r="C190" s="33">
+        <f>'Individual Treasure'!B21</f>
+        <v>2837.3166689405625</v>
+      </c>
+      <c r="D190" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="E190" s="56"/>
+      <c r="F190" s="34">
+        <f>SUMPRODUCT(C185:C189,F185:F189)</f>
+        <v>2850</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="101">
-    <mergeCell ref="G22:L22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="A31:L31"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:F33"/>
+  <mergeCells count="119">
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="D180:E180"/>
+    <mergeCell ref="A181:L181"/>
+    <mergeCell ref="A182:F182"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="D183:F183"/>
+    <mergeCell ref="A190:B190"/>
+    <mergeCell ref="D190:E190"/>
+    <mergeCell ref="A161:L161"/>
+    <mergeCell ref="A162:F162"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="D163:F163"/>
+    <mergeCell ref="A170:B170"/>
+    <mergeCell ref="D170:E170"/>
+    <mergeCell ref="A171:L171"/>
+    <mergeCell ref="A172:F172"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="D173:F173"/>
+    <mergeCell ref="A151:L151"/>
+    <mergeCell ref="A152:F152"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="D153:F153"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="D160:E160"/>
+    <mergeCell ref="A141:L141"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="D143:F143"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="A131:L131"/>
+    <mergeCell ref="A132:F132"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="D133:F133"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="D140:E140"/>
+    <mergeCell ref="A121:L121"/>
+    <mergeCell ref="A122:F122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D123:F123"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="A111:L111"/>
+    <mergeCell ref="A112:F112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D113:F113"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="A101:L101"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D103:F103"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="A91:L91"/>
+    <mergeCell ref="A92:F92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:F93"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="A81:L81"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="A71:L71"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="A61:L61"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="A51:L51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A41:L41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="D20:E20"/>
@@ -5118,78 +5802,15 @@
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A51:L51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="A41:L41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="A71:L71"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="A61:L61"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="A91:L91"/>
-    <mergeCell ref="A92:F92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:F93"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="A81:L81"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="A111:L111"/>
-    <mergeCell ref="A112:F112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D113:F113"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D120:E120"/>
-    <mergeCell ref="A101:L101"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D103:F103"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="A131:L131"/>
-    <mergeCell ref="A132:F132"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="D133:F133"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="D140:E140"/>
-    <mergeCell ref="A121:L121"/>
-    <mergeCell ref="A122:F122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D123:F123"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="A151:L151"/>
-    <mergeCell ref="A152:F152"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="D153:F153"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="D160:E160"/>
-    <mergeCell ref="A141:L141"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="D143:F143"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="G22:L22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="A31:L31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:F33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5260,7 +5881,7 @@
       <c r="W1" s="63"/>
     </row>
     <row r="2" spans="1:23" s="14" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="48" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="64"/>
@@ -6179,7 +6800,7 @@
       <c r="W1" s="63"/>
     </row>
     <row r="2" spans="1:23" s="14" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="48" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="64"/>
@@ -7098,7 +7719,7 @@
       <c r="W1" s="63"/>
     </row>
     <row r="2" spans="1:23" s="14" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="48" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="64"/>

</xml_diff>

<commit_message>
Update individual treasure averages
</commit_message>
<xml_diff>
--- a/Individual Treasure Averages.xlsx
+++ b/Individual Treasure Averages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72182FB-E997-4778-9D16-F612EC0E4FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD63BF2-B39B-440B-BF2F-D5782B389F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" tabRatio="616" activeTab="1" xr2:uid="{5E3698F5-01A8-41EE-A738-BAB99CC962C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="616" activeTab="1" xr2:uid="{5E3698F5-01A8-41EE-A738-BAB99CC962C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Individual Treasure" sheetId="1" r:id="rId1"/>
@@ -25,23 +25,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="88">
   <si>
     <t>Individual gp Per Formula</t>
   </si>
@@ -300,6 +289,12 @@
   <si>
     <t>CR 16: Humanoid</t>
   </si>
+  <si>
+    <t>CR 7: Large Creature</t>
+  </si>
+  <si>
+    <t>CR 10: Large Creature</t>
+  </si>
 </sst>
 </file>
 
@@ -542,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -677,6 +672,21 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -696,21 +706,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -736,6 +731,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1660,8 +1658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD8D082-213D-4692-B6C5-868C3C1BDB24}">
   <dimension ref="A1:AD190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="L178" sqref="L178"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,7 +1678,7 @@
     <col min="12" max="12" width="11.5703125" style="8" customWidth="1"/>
     <col min="13" max="13" width="13.140625" style="8" customWidth="1"/>
     <col min="14" max="14" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="8"/>
+    <col min="15" max="15" width="9.140625" style="8" customWidth="1"/>
     <col min="16" max="16" width="10.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.5703125" style="8" customWidth="1"/>
     <col min="18" max="18" width="13.140625" style="8" customWidth="1"/>
@@ -1700,20 +1698,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
       <c r="Z1" s="39"/>
       <c r="AA1" s="39"/>
       <c r="AB1" s="39"/>
@@ -1755,10 +1753,10 @@
       <c r="AD2" s="37"/>
     </row>
     <row r="3" spans="1:30" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="49"/>
+      <c r="B3" s="54"/>
       <c r="C3" s="21">
         <v>3</v>
       </c>
@@ -1953,18 +1951,18 @@
       </c>
     </row>
     <row r="10" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="54"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="33">
         <f>'Individual Treasure'!B3</f>
         <v>1.0794007754789445</v>
       </c>
-      <c r="D10" s="55" t="s">
+      <c r="D10" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="56"/>
+      <c r="E10" s="49"/>
       <c r="F10" s="34">
         <f>SUMPRODUCT(C5:C9,F5:F9)</f>
         <v>1</v>
@@ -1990,20 +1988,20 @@
       <c r="AD10" s="13"/>
     </row>
     <row r="11" spans="1:30" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
       <c r="Z11" s="39"/>
       <c r="AA11" s="39"/>
       <c r="AB11" s="39"/>
@@ -2011,14 +2009,14 @@
       <c r="AD11" s="39"/>
     </row>
     <row r="12" spans="1:30" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="47"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="52"/>
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
       <c r="I12" s="37"/>
@@ -2045,18 +2043,18 @@
       <c r="AD12" s="37"/>
     </row>
     <row r="13" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="49"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="21">
         <v>3</v>
       </c>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="51"/>
-      <c r="F13" s="52"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="57"/>
       <c r="G13" s="38"/>
       <c r="H13" s="38"/>
       <c r="I13" s="36"/>
@@ -2213,18 +2211,18 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="54"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="33">
         <f>'Individual Treasure'!B4</f>
         <v>1.6717350674697367</v>
       </c>
-      <c r="D20" s="55" t="s">
+      <c r="D20" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="56"/>
+      <c r="E20" s="49"/>
       <c r="F20" s="34">
         <f>SUMPRODUCT(C15:C19,F15:F19)</f>
         <v>1.6750000000000003</v>
@@ -2233,64 +2231,64 @@
       <c r="K20" s="13"/>
     </row>
     <row r="21" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="57" t="s">
+      <c r="A21" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="57"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="57"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="57"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
     </row>
     <row r="22" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="46" t="s">
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="47"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="52"/>
     </row>
     <row r="23" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="48" t="s">
+      <c r="A23" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="49"/>
+      <c r="B23" s="54"/>
       <c r="C23" s="21">
         <v>3</v>
       </c>
-      <c r="D23" s="50" t="s">
+      <c r="D23" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="51"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="48" t="s">
+      <c r="E23" s="56"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="H23" s="49"/>
+      <c r="H23" s="54"/>
       <c r="I23" s="21">
         <v>3</v>
       </c>
-      <c r="J23" s="50" t="s">
+      <c r="J23" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="K23" s="51"/>
-      <c r="L23" s="52"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="57"/>
     </row>
     <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="42" t="s">
@@ -2553,78 +2551,78 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="54"/>
+      <c r="B30" s="47"/>
       <c r="C30" s="33">
         <f>'Individual Treasure'!B5</f>
         <v>2.5891199999999999</v>
       </c>
-      <c r="D30" s="55" t="s">
+      <c r="D30" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="56"/>
+      <c r="E30" s="49"/>
       <c r="F30" s="34">
         <f>SUMPRODUCT(C25:C29,F25:F29)</f>
         <v>2.5750000000000002</v>
       </c>
-      <c r="G30" s="53" t="s">
+      <c r="G30" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="H30" s="54"/>
+      <c r="H30" s="47"/>
       <c r="I30" s="33">
         <f>'Individual Treasure'!B5</f>
         <v>2.5891199999999999</v>
       </c>
-      <c r="J30" s="55" t="s">
+      <c r="J30" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="K30" s="56"/>
+      <c r="K30" s="49"/>
       <c r="L30" s="34">
         <f>SUMPRODUCT(I25:I29,L25:L29)</f>
         <v>2.5499999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="57" t="s">
+      <c r="A31" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="57"/>
-      <c r="J31" s="57"/>
-      <c r="K31" s="57"/>
-      <c r="L31" s="57"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="50"/>
+      <c r="L31" s="50"/>
     </row>
     <row r="32" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A32" s="46" t="s">
+      <c r="A32" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="47"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="52"/>
     </row>
     <row r="33" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="48" t="s">
+      <c r="A33" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="49"/>
+      <c r="B33" s="54"/>
       <c r="C33" s="21">
         <v>3</v>
       </c>
-      <c r="D33" s="50" t="s">
+      <c r="D33" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E33" s="51"/>
-      <c r="F33" s="52"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="57"/>
     </row>
     <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="42" t="s">
@@ -2763,62 +2761,62 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="53" t="s">
+      <c r="A40" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="54"/>
+      <c r="B40" s="47"/>
       <c r="C40" s="33">
         <f>'Individual Treasure'!B6</f>
         <v>4.0099310619512103</v>
       </c>
-      <c r="D40" s="55" t="s">
+      <c r="D40" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="56"/>
+      <c r="E40" s="49"/>
       <c r="F40" s="34">
         <f>SUMPRODUCT(C35:C39,F35:F39)</f>
         <v>4.05</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="57" t="s">
+      <c r="A41" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="57"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="57"/>
-      <c r="E41" s="57"/>
-      <c r="F41" s="57"/>
-      <c r="G41" s="57"/>
-      <c r="H41" s="57"/>
-      <c r="I41" s="57"/>
-      <c r="J41" s="57"/>
-      <c r="K41" s="57"/>
-      <c r="L41" s="57"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="50"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="50"/>
+      <c r="K41" s="50"/>
+      <c r="L41" s="50"/>
     </row>
     <row r="42" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="46"/>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="47"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="52"/>
     </row>
     <row r="43" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="48" t="s">
+      <c r="A43" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="49"/>
+      <c r="B43" s="54"/>
       <c r="C43" s="21">
         <v>3</v>
       </c>
-      <c r="D43" s="50" t="s">
+      <c r="D43" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E43" s="51"/>
-      <c r="F43" s="52"/>
+      <c r="E43" s="56"/>
+      <c r="F43" s="57"/>
     </row>
     <row r="44" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="42" t="s">
@@ -2957,62 +2955,62 @@
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="53" t="s">
+      <c r="A50" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="54"/>
+      <c r="B50" s="47"/>
       <c r="C50" s="33">
         <f>'Individual Treasure'!B7</f>
         <v>6.2104294592761873</v>
       </c>
-      <c r="D50" s="55" t="s">
+      <c r="D50" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E50" s="56"/>
+      <c r="E50" s="49"/>
       <c r="F50" s="34">
         <f>SUMPRODUCT(C45:C49,F45:F49)</f>
         <v>6.2000000000000011</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="57" t="s">
+      <c r="A51" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="57"/>
-      <c r="C51" s="57"/>
-      <c r="D51" s="57"/>
-      <c r="E51" s="57"/>
-      <c r="F51" s="57"/>
-      <c r="G51" s="57"/>
-      <c r="H51" s="57"/>
-      <c r="I51" s="57"/>
-      <c r="J51" s="57"/>
-      <c r="K51" s="57"/>
-      <c r="L51" s="57"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="50"/>
+      <c r="H51" s="50"/>
+      <c r="I51" s="50"/>
+      <c r="J51" s="50"/>
+      <c r="K51" s="50"/>
+      <c r="L51" s="50"/>
     </row>
     <row r="52" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A52" s="46" t="s">
+      <c r="A52" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="B52" s="46"/>
-      <c r="C52" s="46"/>
-      <c r="D52" s="46"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="47"/>
+      <c r="B52" s="51"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="51"/>
+      <c r="F52" s="52"/>
     </row>
     <row r="53" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="48" t="s">
+      <c r="A53" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B53" s="49"/>
+      <c r="B53" s="54"/>
       <c r="C53" s="21">
         <v>3</v>
       </c>
-      <c r="D53" s="50" t="s">
+      <c r="D53" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E53" s="51"/>
-      <c r="F53" s="52"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="57"/>
     </row>
     <row r="54" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="42" t="s">
@@ -3151,62 +3149,62 @@
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="53" t="s">
+      <c r="A60" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B60" s="54"/>
+      <c r="B60" s="47"/>
       <c r="C60" s="33">
         <f>'Individual Treasure'!B8</f>
         <v>9.6184780917100969</v>
       </c>
-      <c r="D60" s="55" t="s">
+      <c r="D60" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E60" s="56"/>
+      <c r="E60" s="49"/>
       <c r="F60" s="34">
         <f>SUMPRODUCT(C55:C59,F55:F59)</f>
         <v>9.6000000000000014</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="57" t="s">
+      <c r="A61" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="57"/>
-      <c r="C61" s="57"/>
-      <c r="D61" s="57"/>
-      <c r="E61" s="57"/>
-      <c r="F61" s="57"/>
-      <c r="G61" s="57"/>
-      <c r="H61" s="57"/>
-      <c r="I61" s="57"/>
-      <c r="J61" s="57"/>
-      <c r="K61" s="57"/>
-      <c r="L61" s="57"/>
+      <c r="B61" s="50"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="50"/>
+      <c r="E61" s="50"/>
+      <c r="F61" s="50"/>
+      <c r="G61" s="50"/>
+      <c r="H61" s="50"/>
+      <c r="I61" s="50"/>
+      <c r="J61" s="50"/>
+      <c r="K61" s="50"/>
+      <c r="L61" s="50"/>
     </row>
     <row r="62" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A62" s="46" t="s">
+      <c r="A62" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="B62" s="46"/>
-      <c r="C62" s="46"/>
-      <c r="D62" s="46"/>
-      <c r="E62" s="46"/>
-      <c r="F62" s="47"/>
+      <c r="B62" s="51"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="51"/>
+      <c r="E62" s="51"/>
+      <c r="F62" s="52"/>
     </row>
     <row r="63" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="48" t="s">
+      <c r="A63" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B63" s="49"/>
+      <c r="B63" s="54"/>
       <c r="C63" s="21">
         <v>3</v>
       </c>
-      <c r="D63" s="50" t="s">
+      <c r="D63" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E63" s="51"/>
-      <c r="F63" s="52"/>
+      <c r="E63" s="56"/>
+      <c r="F63" s="57"/>
     </row>
     <row r="64" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="42" t="s">
@@ -3345,62 +3343,62 @@
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="53" t="s">
+      <c r="A70" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B70" s="54"/>
+      <c r="B70" s="47"/>
       <c r="C70" s="33">
         <f>'Individual Treasure'!B9</f>
         <v>14.89673482443669</v>
       </c>
-      <c r="D70" s="55" t="s">
+      <c r="D70" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E70" s="56"/>
+      <c r="E70" s="49"/>
       <c r="F70" s="34">
         <f>SUMPRODUCT(C65:C69,F65:F69)</f>
         <v>14.900000000000002</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="57" t="s">
+      <c r="A71" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="B71" s="57"/>
-      <c r="C71" s="57"/>
-      <c r="D71" s="57"/>
-      <c r="E71" s="57"/>
-      <c r="F71" s="57"/>
-      <c r="G71" s="57"/>
-      <c r="H71" s="57"/>
-      <c r="I71" s="57"/>
-      <c r="J71" s="57"/>
-      <c r="K71" s="57"/>
-      <c r="L71" s="57"/>
+      <c r="B71" s="50"/>
+      <c r="C71" s="50"/>
+      <c r="D71" s="50"/>
+      <c r="E71" s="50"/>
+      <c r="F71" s="50"/>
+      <c r="G71" s="50"/>
+      <c r="H71" s="50"/>
+      <c r="I71" s="50"/>
+      <c r="J71" s="50"/>
+      <c r="K71" s="50"/>
+      <c r="L71" s="50"/>
     </row>
     <row r="72" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A72" s="46" t="s">
+      <c r="A72" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B72" s="46"/>
-      <c r="C72" s="46"/>
-      <c r="D72" s="46"/>
-      <c r="E72" s="46"/>
-      <c r="F72" s="47"/>
+      <c r="B72" s="51"/>
+      <c r="C72" s="51"/>
+      <c r="D72" s="51"/>
+      <c r="E72" s="51"/>
+      <c r="F72" s="52"/>
     </row>
     <row r="73" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="48" t="s">
+      <c r="A73" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B73" s="49"/>
+      <c r="B73" s="54"/>
       <c r="C73" s="21">
         <v>5</v>
       </c>
-      <c r="D73" s="50" t="s">
+      <c r="D73" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E73" s="51"/>
-      <c r="F73" s="52"/>
+      <c r="E73" s="56"/>
+      <c r="F73" s="57"/>
     </row>
     <row r="74" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="42" t="s">
@@ -3539,62 +3537,62 @@
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" s="53" t="s">
+      <c r="A80" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B80" s="54"/>
+      <c r="B80" s="47"/>
       <c r="C80" s="33">
         <f>'Individual Treasure'!B10</f>
         <v>23.071499078512772</v>
       </c>
-      <c r="D80" s="55" t="s">
+      <c r="D80" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E80" s="56"/>
+      <c r="E80" s="49"/>
       <c r="F80" s="34">
         <f>SUMPRODUCT(C75:C79,F75:F79)</f>
         <v>23</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="57" t="s">
+      <c r="A81" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="B81" s="57"/>
-      <c r="C81" s="57"/>
-      <c r="D81" s="57"/>
-      <c r="E81" s="57"/>
-      <c r="F81" s="57"/>
-      <c r="G81" s="57"/>
-      <c r="H81" s="57"/>
-      <c r="I81" s="57"/>
-      <c r="J81" s="57"/>
-      <c r="K81" s="57"/>
-      <c r="L81" s="57"/>
+      <c r="B81" s="50"/>
+      <c r="C81" s="50"/>
+      <c r="D81" s="50"/>
+      <c r="E81" s="50"/>
+      <c r="F81" s="50"/>
+      <c r="G81" s="50"/>
+      <c r="H81" s="50"/>
+      <c r="I81" s="50"/>
+      <c r="J81" s="50"/>
+      <c r="K81" s="50"/>
+      <c r="L81" s="50"/>
     </row>
     <row r="82" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A82" s="46" t="s">
+      <c r="A82" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="B82" s="46"/>
-      <c r="C82" s="46"/>
-      <c r="D82" s="46"/>
-      <c r="E82" s="46"/>
-      <c r="F82" s="47"/>
+      <c r="B82" s="51"/>
+      <c r="C82" s="51"/>
+      <c r="D82" s="51"/>
+      <c r="E82" s="51"/>
+      <c r="F82" s="52"/>
     </row>
     <row r="83" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="48" t="s">
+      <c r="A83" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B83" s="49"/>
+      <c r="B83" s="54"/>
       <c r="C83" s="21">
         <v>5</v>
       </c>
-      <c r="D83" s="50" t="s">
+      <c r="D83" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E83" s="51"/>
-      <c r="F83" s="52"/>
+      <c r="E83" s="56"/>
+      <c r="F83" s="57"/>
     </row>
     <row r="84" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="42" t="s">
@@ -3733,64 +3731,84 @@
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A90" s="53" t="s">
+      <c r="A90" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B90" s="54"/>
+      <c r="B90" s="47"/>
       <c r="C90" s="33">
         <f>'Individual Treasure'!B11</f>
         <v>35.732264553480377</v>
       </c>
-      <c r="D90" s="55" t="s">
+      <c r="D90" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E90" s="56"/>
+      <c r="E90" s="49"/>
       <c r="F90" s="34">
         <f>SUMPRODUCT(C85:C89,F85:F89)</f>
         <v>35</v>
       </c>
     </row>
     <row r="91" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="57" t="s">
+      <c r="A91" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B91" s="57"/>
-      <c r="C91" s="57"/>
-      <c r="D91" s="57"/>
-      <c r="E91" s="57"/>
-      <c r="F91" s="57"/>
-      <c r="G91" s="57"/>
-      <c r="H91" s="57"/>
-      <c r="I91" s="57"/>
-      <c r="J91" s="57"/>
-      <c r="K91" s="57"/>
-      <c r="L91" s="57"/>
+      <c r="B91" s="50"/>
+      <c r="C91" s="50"/>
+      <c r="D91" s="50"/>
+      <c r="E91" s="50"/>
+      <c r="F91" s="50"/>
+      <c r="G91" s="50"/>
+      <c r="H91" s="50"/>
+      <c r="I91" s="50"/>
+      <c r="J91" s="50"/>
+      <c r="K91" s="50"/>
+      <c r="L91" s="50"/>
     </row>
     <row r="92" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A92" s="46" t="s">
+      <c r="A92" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="B92" s="46"/>
-      <c r="C92" s="46"/>
-      <c r="D92" s="46"/>
-      <c r="E92" s="46"/>
-      <c r="F92" s="47"/>
+      <c r="B92" s="51"/>
+      <c r="C92" s="51"/>
+      <c r="D92" s="51"/>
+      <c r="E92" s="51"/>
+      <c r="F92" s="52"/>
+      <c r="G92" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="H92" s="51"/>
+      <c r="I92" s="51"/>
+      <c r="J92" s="51"/>
+      <c r="K92" s="51"/>
+      <c r="L92" s="52"/>
     </row>
     <row r="93" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="48" t="s">
+      <c r="A93" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B93" s="49"/>
+      <c r="B93" s="54"/>
       <c r="C93" s="21">
         <v>5</v>
       </c>
-      <c r="D93" s="50" t="s">
+      <c r="D93" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E93" s="51"/>
-      <c r="F93" s="52"/>
-    </row>
-    <row r="94" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="E93" s="56"/>
+      <c r="F93" s="57"/>
+      <c r="G93" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="H93" s="54"/>
+      <c r="I93" s="21">
+        <v>5</v>
+      </c>
+      <c r="J93" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="K93" s="56"/>
+      <c r="L93" s="57"/>
+    </row>
+    <row r="94" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="42" t="s">
         <v>9</v>
       </c>
@@ -3807,6 +3825,24 @@
         <v>24</v>
       </c>
       <c r="F94" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G94" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H94" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I94" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="J94" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="K94" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="L94" s="17" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3832,6 +3868,27 @@
         <f>D95*E95</f>
         <v>15</v>
       </c>
+      <c r="G95" s="43">
+        <f>I93+1</f>
+        <v>6</v>
+      </c>
+      <c r="H95" s="8">
+        <v>7</v>
+      </c>
+      <c r="I95" s="31">
+        <f>((H95-G95+1)*0.05)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J95" s="18">
+        <v>3</v>
+      </c>
+      <c r="K95" s="8">
+        <v>5</v>
+      </c>
+      <c r="L95" s="19">
+        <f>J95*K95</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="43">
@@ -3855,10 +3912,31 @@
         <f t="shared" ref="F96:F99" si="31">D96*E96</f>
         <v>30</v>
       </c>
+      <c r="G96" s="43">
+        <f>H95+1</f>
+        <v>8</v>
+      </c>
+      <c r="H96" s="8">
+        <v>10</v>
+      </c>
+      <c r="I96" s="31">
+        <f t="shared" ref="I96:I99" si="32">((H96-G96+1)*0.05)</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="J96" s="18">
+        <v>5</v>
+      </c>
+      <c r="K96" s="8">
+        <v>5</v>
+      </c>
+      <c r="L96" s="19">
+        <f t="shared" ref="L96:L99" si="33">J96*K96</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="43">
-        <f t="shared" ref="A97:A99" si="32">B96+1</f>
+        <f t="shared" ref="A97:A99" si="34">B96+1</f>
         <v>16</v>
       </c>
       <c r="B97" s="8">
@@ -3878,10 +3956,31 @@
         <f t="shared" si="31"/>
         <v>50</v>
       </c>
+      <c r="G97" s="43">
+        <f t="shared" ref="G97:G99" si="35">H96+1</f>
+        <v>11</v>
+      </c>
+      <c r="H97" s="8">
+        <v>16</v>
+      </c>
+      <c r="I97" s="31">
+        <f t="shared" si="32"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="J97" s="18">
+        <v>5</v>
+      </c>
+      <c r="K97" s="8">
+        <v>10</v>
+      </c>
+      <c r="L97" s="19">
+        <f t="shared" si="33"/>
+        <v>50</v>
+      </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="43">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>21</v>
       </c>
       <c r="B98" s="8">
@@ -3901,10 +4000,31 @@
         <f t="shared" si="31"/>
         <v>100</v>
       </c>
+      <c r="G98" s="43">
+        <f t="shared" si="35"/>
+        <v>17</v>
+      </c>
+      <c r="H98" s="8">
+        <v>22</v>
+      </c>
+      <c r="I98" s="31">
+        <f t="shared" si="32"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="J98" s="18">
+        <v>7</v>
+      </c>
+      <c r="K98" s="8">
+        <v>10</v>
+      </c>
+      <c r="L98" s="19">
+        <f t="shared" si="33"/>
+        <v>70</v>
+      </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="43">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>25</v>
       </c>
       <c r="B99" s="44">
@@ -3925,64 +4045,102 @@
         <f t="shared" si="31"/>
         <v>200</v>
       </c>
+      <c r="G99" s="43">
+        <f t="shared" si="35"/>
+        <v>23</v>
+      </c>
+      <c r="H99" s="44">
+        <f>20+I93</f>
+        <v>25</v>
+      </c>
+      <c r="I99" s="31">
+        <f t="shared" si="32"/>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="J99" s="20">
+        <v>5</v>
+      </c>
+      <c r="K99" s="28">
+        <v>20</v>
+      </c>
+      <c r="L99" s="22">
+        <f t="shared" si="33"/>
+        <v>100</v>
+      </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A100" s="53" t="s">
+      <c r="A100" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B100" s="54"/>
+      <c r="B100" s="47"/>
       <c r="C100" s="33">
         <f>'Individual Treasure'!B12</f>
         <v>55.340778931397217</v>
       </c>
-      <c r="D100" s="55" t="s">
+      <c r="D100" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E100" s="56"/>
+      <c r="E100" s="49"/>
       <c r="F100" s="34">
         <f>SUMPRODUCT(C95:C99,F95:F99)</f>
         <v>55.25</v>
       </c>
+      <c r="G100" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="H100" s="47"/>
+      <c r="I100" s="33">
+        <f>'Individual Treasure'!B12</f>
+        <v>55.340778931397217</v>
+      </c>
+      <c r="J100" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="K100" s="49"/>
+      <c r="L100" s="34">
+        <f>SUMPRODUCT(I95:I99,L95:L99)</f>
+        <v>56.25</v>
+      </c>
     </row>
     <row r="101" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A101" s="57" t="s">
+      <c r="A101" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="B101" s="57"/>
-      <c r="C101" s="57"/>
-      <c r="D101" s="57"/>
-      <c r="E101" s="57"/>
-      <c r="F101" s="57"/>
-      <c r="G101" s="57"/>
-      <c r="H101" s="57"/>
-      <c r="I101" s="57"/>
-      <c r="J101" s="57"/>
-      <c r="K101" s="57"/>
-      <c r="L101" s="57"/>
+      <c r="B101" s="50"/>
+      <c r="C101" s="50"/>
+      <c r="D101" s="50"/>
+      <c r="E101" s="50"/>
+      <c r="F101" s="50"/>
+      <c r="G101" s="50"/>
+      <c r="H101" s="50"/>
+      <c r="I101" s="50"/>
+      <c r="J101" s="50"/>
+      <c r="K101" s="50"/>
+      <c r="L101" s="50"/>
     </row>
     <row r="102" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A102" s="46" t="s">
+      <c r="A102" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="B102" s="46"/>
-      <c r="C102" s="46"/>
-      <c r="D102" s="46"/>
-      <c r="E102" s="46"/>
-      <c r="F102" s="47"/>
-    </row>
-    <row r="103" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="48" t="s">
+      <c r="B102" s="51"/>
+      <c r="C102" s="51"/>
+      <c r="D102" s="51"/>
+      <c r="E102" s="51"/>
+      <c r="F102" s="52"/>
+    </row>
+    <row r="103" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B103" s="49"/>
+      <c r="B103" s="54"/>
       <c r="C103" s="21">
         <v>5</v>
       </c>
-      <c r="D103" s="50" t="s">
+      <c r="D103" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E103" s="51"/>
-      <c r="F103" s="52"/>
+      <c r="E103" s="56"/>
+      <c r="F103" s="57"/>
     </row>
     <row r="104" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="42" t="s">
@@ -4036,7 +4194,7 @@
         <v>12</v>
       </c>
       <c r="C106" s="31">
-        <f t="shared" ref="C106:C109" si="33">((B106-A106+1)*0.05)</f>
+        <f t="shared" ref="C106:C109" si="36">((B106-A106+1)*0.05)</f>
         <v>0.25</v>
       </c>
       <c r="D106" s="18">
@@ -4046,20 +4204,20 @@
         <v>20</v>
       </c>
       <c r="F106" s="19">
-        <f t="shared" ref="F106:F109" si="34">D106*E106</f>
+        <f t="shared" ref="F106:F109" si="37">D106*E106</f>
         <v>40</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="43">
-        <f t="shared" ref="A107:A109" si="35">B106+1</f>
+        <f t="shared" ref="A107:A109" si="38">B106+1</f>
         <v>13</v>
       </c>
       <c r="B107" s="8">
         <v>17</v>
       </c>
       <c r="C107" s="31">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>0.25</v>
       </c>
       <c r="D107" s="18">
@@ -4069,20 +4227,20 @@
         <v>50</v>
       </c>
       <c r="F107" s="19">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>50</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="43">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>18</v>
       </c>
       <c r="B108" s="8">
         <v>21</v>
       </c>
       <c r="C108" s="31">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>0.2</v>
       </c>
       <c r="D108" s="18">
@@ -4092,13 +4250,13 @@
         <v>50</v>
       </c>
       <c r="F108" s="19">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>100</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="43">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>22</v>
       </c>
       <c r="B109" s="44">
@@ -4106,7 +4264,7 @@
         <v>25</v>
       </c>
       <c r="C109" s="31">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>0.2</v>
       </c>
       <c r="D109" s="20">
@@ -4116,67 +4274,67 @@
         <v>100</v>
       </c>
       <c r="F109" s="22">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>200</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A110" s="53" t="s">
+    <row r="110" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B110" s="54"/>
+      <c r="B110" s="47"/>
       <c r="C110" s="33">
         <f>'Individual Treasure'!B13</f>
         <v>85.709703849023938</v>
       </c>
-      <c r="D110" s="55" t="s">
+      <c r="D110" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E110" s="56"/>
+      <c r="E110" s="49"/>
       <c r="F110" s="34">
         <f>SUMPRODUCT(C105:C109,F105:F109)</f>
         <v>85.5</v>
       </c>
     </row>
     <row r="111" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A111" s="57" t="s">
+      <c r="A111" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="B111" s="57"/>
-      <c r="C111" s="57"/>
-      <c r="D111" s="57"/>
-      <c r="E111" s="57"/>
-      <c r="F111" s="57"/>
-      <c r="G111" s="57"/>
-      <c r="H111" s="57"/>
-      <c r="I111" s="57"/>
-      <c r="J111" s="57"/>
-      <c r="K111" s="57"/>
-      <c r="L111" s="57"/>
+      <c r="B111" s="50"/>
+      <c r="C111" s="50"/>
+      <c r="D111" s="50"/>
+      <c r="E111" s="50"/>
+      <c r="F111" s="50"/>
+      <c r="G111" s="50"/>
+      <c r="H111" s="50"/>
+      <c r="I111" s="50"/>
+      <c r="J111" s="50"/>
+      <c r="K111" s="50"/>
+      <c r="L111" s="50"/>
     </row>
     <row r="112" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A112" s="46" t="s">
+      <c r="A112" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="B112" s="46"/>
-      <c r="C112" s="46"/>
-      <c r="D112" s="46"/>
-      <c r="E112" s="46"/>
-      <c r="F112" s="47"/>
+      <c r="B112" s="51"/>
+      <c r="C112" s="51"/>
+      <c r="D112" s="51"/>
+      <c r="E112" s="51"/>
+      <c r="F112" s="52"/>
     </row>
     <row r="113" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="48" t="s">
+      <c r="A113" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B113" s="49"/>
+      <c r="B113" s="54"/>
       <c r="C113" s="21">
         <v>5</v>
       </c>
-      <c r="D113" s="50" t="s">
+      <c r="D113" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E113" s="51"/>
-      <c r="F113" s="52"/>
+      <c r="E113" s="56"/>
+      <c r="F113" s="57"/>
     </row>
     <row r="114" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="42" t="s">
@@ -4230,7 +4388,7 @@
         <v>12</v>
       </c>
       <c r="C116" s="31">
-        <f t="shared" ref="C116:C119" si="36">((B116-A116+1)*0.05)</f>
+        <f t="shared" ref="C116:C119" si="39">((B116-A116+1)*0.05)</f>
         <v>0.25</v>
       </c>
       <c r="D116" s="18">
@@ -4240,20 +4398,20 @@
         <v>20</v>
       </c>
       <c r="F116" s="19">
-        <f t="shared" ref="F116:F119" si="37">D116*E116</f>
+        <f t="shared" ref="F116:F119" si="40">D116*E116</f>
         <v>60</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="43">
-        <f t="shared" ref="A117:A119" si="38">B116+1</f>
+        <f t="shared" ref="A117:A119" si="41">B116+1</f>
         <v>13</v>
       </c>
       <c r="B117" s="8">
         <v>17</v>
       </c>
       <c r="C117" s="31">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.25</v>
       </c>
       <c r="D117" s="18">
@@ -4263,20 +4421,20 @@
         <v>50</v>
       </c>
       <c r="F117" s="19">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>100</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>18</v>
       </c>
       <c r="B118" s="8">
         <v>24</v>
       </c>
       <c r="C118" s="31">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.35000000000000003</v>
       </c>
       <c r="D118" s="18">
@@ -4286,13 +4444,13 @@
         <v>100</v>
       </c>
       <c r="F118" s="19">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>200</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>25</v>
       </c>
       <c r="B119" s="44">
@@ -4300,7 +4458,7 @@
         <v>25</v>
       </c>
       <c r="C119" s="31">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.05</v>
       </c>
       <c r="D119" s="20">
@@ -4310,69 +4468,89 @@
         <v>200</v>
       </c>
       <c r="F119" s="22">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>400</v>
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A120" s="53" t="s">
+      <c r="A120" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B120" s="54"/>
+      <c r="B120" s="47"/>
       <c r="C120" s="33">
         <f>'Individual Treasure'!B14</f>
         <v>132.7439453462336</v>
       </c>
-      <c r="D120" s="55" t="s">
+      <c r="D120" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E120" s="56"/>
+      <c r="E120" s="49"/>
       <c r="F120" s="34">
         <f>SUMPRODUCT(C115:C119,F115:F119)</f>
         <v>133</v>
       </c>
     </row>
     <row r="121" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A121" s="57" t="s">
+      <c r="A121" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="B121" s="57"/>
-      <c r="C121" s="57"/>
-      <c r="D121" s="57"/>
-      <c r="E121" s="57"/>
-      <c r="F121" s="57"/>
-      <c r="G121" s="57"/>
-      <c r="H121" s="57"/>
-      <c r="I121" s="57"/>
-      <c r="J121" s="57"/>
-      <c r="K121" s="57"/>
-      <c r="L121" s="57"/>
+      <c r="B121" s="50"/>
+      <c r="C121" s="50"/>
+      <c r="D121" s="50"/>
+      <c r="E121" s="50"/>
+      <c r="F121" s="50"/>
+      <c r="G121" s="50"/>
+      <c r="H121" s="50"/>
+      <c r="I121" s="50"/>
+      <c r="J121" s="50"/>
+      <c r="K121" s="50"/>
+      <c r="L121" s="50"/>
     </row>
     <row r="122" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A122" s="46" t="s">
+      <c r="A122" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="B122" s="46"/>
-      <c r="C122" s="46"/>
-      <c r="D122" s="46"/>
-      <c r="E122" s="46"/>
-      <c r="F122" s="47"/>
-    </row>
-    <row r="123" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A123" s="48" t="s">
+      <c r="B122" s="51"/>
+      <c r="C122" s="51"/>
+      <c r="D122" s="51"/>
+      <c r="E122" s="51"/>
+      <c r="F122" s="52"/>
+      <c r="G122" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="H122" s="51"/>
+      <c r="I122" s="51"/>
+      <c r="J122" s="51"/>
+      <c r="K122" s="51"/>
+      <c r="L122" s="52"/>
+    </row>
+    <row r="123" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B123" s="49"/>
+      <c r="B123" s="54"/>
       <c r="C123" s="21">
         <v>5</v>
       </c>
-      <c r="D123" s="50" t="s">
+      <c r="D123" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E123" s="51"/>
-      <c r="F123" s="52"/>
-    </row>
-    <row r="124" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="E123" s="56"/>
+      <c r="F123" s="57"/>
+      <c r="G123" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="H123" s="54"/>
+      <c r="I123" s="21">
+        <v>5</v>
+      </c>
+      <c r="J123" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="K123" s="56"/>
+      <c r="L123" s="57"/>
+    </row>
+    <row r="124" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="42" t="s">
         <v>9</v>
       </c>
@@ -4389,6 +4567,24 @@
         <v>24</v>
       </c>
       <c r="F124" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G124" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H124" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I124" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="J124" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="K124" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="L124" s="17" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4414,8 +4610,29 @@
         <f>D125*E125</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G125" s="43">
+        <f>I123+1</f>
+        <v>6</v>
+      </c>
+      <c r="H125" s="8">
+        <v>7</v>
+      </c>
+      <c r="I125" s="31">
+        <f>((H125-G125+1)*0.05)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J125" s="18">
+        <v>3</v>
+      </c>
+      <c r="K125" s="8">
+        <v>10</v>
+      </c>
+      <c r="L125" s="19">
+        <f>J125*K125</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="43">
         <f>B125+1</f>
         <v>8</v>
@@ -4424,7 +4641,7 @@
         <v>9</v>
       </c>
       <c r="C126" s="31">
-        <f t="shared" ref="C126:C129" si="39">((B126-A126+1)*0.05)</f>
+        <f t="shared" ref="C126:C129" si="42">((B126-A126+1)*0.05)</f>
         <v>0.1</v>
       </c>
       <c r="D126" s="18">
@@ -4434,20 +4651,41 @@
         <v>50</v>
       </c>
       <c r="F126" s="19">
-        <f t="shared" ref="F126:F129" si="40">D126*E126</f>
+        <f t="shared" ref="F126:F129" si="43">D126*E126</f>
         <v>100</v>
+      </c>
+      <c r="G126" s="43">
+        <f>H125+1</f>
+        <v>8</v>
+      </c>
+      <c r="H126" s="8">
+        <v>12</v>
+      </c>
+      <c r="I126" s="31">
+        <f t="shared" ref="I126:I129" si="44">((H126-G126+1)*0.05)</f>
+        <v>0.25</v>
+      </c>
+      <c r="J126" s="18">
+        <v>3</v>
+      </c>
+      <c r="K126" s="8">
+        <v>20</v>
+      </c>
+      <c r="L126" s="19">
+        <f t="shared" ref="L126:L129" si="45">J126*K126</f>
+        <v>60</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="43">
-        <f t="shared" ref="A127:A129" si="41">B126+1</f>
+        <f t="shared" ref="A127:A129" si="46">B126+1</f>
         <v>10</v>
       </c>
       <c r="B127" s="8">
         <v>13</v>
       </c>
       <c r="C127" s="31">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>0.2</v>
       </c>
       <c r="D127" s="18">
@@ -4457,20 +4695,41 @@
         <v>50</v>
       </c>
       <c r="F127" s="19">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
+        <v>150</v>
+      </c>
+      <c r="G127" s="43">
+        <f t="shared" ref="G127:G129" si="47">H126+1</f>
+        <v>13</v>
+      </c>
+      <c r="H127" s="8">
+        <v>17</v>
+      </c>
+      <c r="I127" s="31">
+        <f t="shared" si="44"/>
+        <v>0.25</v>
+      </c>
+      <c r="J127" s="18">
+        <v>3</v>
+      </c>
+      <c r="K127" s="8">
+        <v>50</v>
+      </c>
+      <c r="L127" s="19">
+        <f t="shared" si="45"/>
         <v>150</v>
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="43">
-        <f t="shared" si="41"/>
+        <f t="shared" si="46"/>
         <v>14</v>
       </c>
       <c r="B128" s="8">
         <v>21</v>
       </c>
       <c r="C128" s="31">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>0.4</v>
       </c>
       <c r="D128" s="18">
@@ -4480,13 +4739,34 @@
         <v>100</v>
       </c>
       <c r="F128" s="19">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>200</v>
+      </c>
+      <c r="G128" s="43">
+        <f t="shared" si="47"/>
+        <v>18</v>
+      </c>
+      <c r="H128" s="8">
+        <v>21</v>
+      </c>
+      <c r="I128" s="31">
+        <f t="shared" si="44"/>
+        <v>0.2</v>
+      </c>
+      <c r="J128" s="18">
+        <v>5</v>
+      </c>
+      <c r="K128" s="8">
+        <v>50</v>
+      </c>
+      <c r="L128" s="19">
+        <f t="shared" si="45"/>
+        <v>250</v>
       </c>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="43">
-        <f t="shared" si="41"/>
+        <f t="shared" si="46"/>
         <v>22</v>
       </c>
       <c r="B129" s="44">
@@ -4494,7 +4774,7 @@
         <v>25</v>
       </c>
       <c r="C129" s="31">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>0.2</v>
       </c>
       <c r="D129" s="20">
@@ -4504,67 +4784,105 @@
         <v>200</v>
       </c>
       <c r="F129" s="22">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>400</v>
       </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A130" s="53" t="s">
+      <c r="G129" s="43">
+        <f t="shared" si="47"/>
+        <v>22</v>
+      </c>
+      <c r="H129" s="44">
+        <f>20+I123</f>
+        <v>25</v>
+      </c>
+      <c r="I129" s="31">
+        <f t="shared" si="44"/>
+        <v>0.2</v>
+      </c>
+      <c r="J129" s="20">
+        <v>5</v>
+      </c>
+      <c r="K129" s="28">
+        <v>100</v>
+      </c>
+      <c r="L129" s="22">
+        <f t="shared" si="45"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B130" s="54"/>
+      <c r="B130" s="47"/>
       <c r="C130" s="33">
         <f>'Individual Treasure'!B15</f>
         <v>205.58879840633722</v>
       </c>
-      <c r="D130" s="55" t="s">
+      <c r="D130" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E130" s="56"/>
+      <c r="E130" s="49"/>
       <c r="F130" s="34">
         <f>SUMPRODUCT(C125:C129,F125:F129)</f>
         <v>205</v>
       </c>
+      <c r="G130" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="H130" s="47"/>
+      <c r="I130" s="33">
+        <f>'Individual Treasure'!B15</f>
+        <v>205.58879840633722</v>
+      </c>
+      <c r="J130" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="K130" s="49"/>
+      <c r="L130" s="34">
+        <f>SUMPRODUCT(I125:I129,L125:L129)</f>
+        <v>205.5</v>
+      </c>
     </row>
     <row r="131" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A131" s="57" t="s">
+      <c r="A131" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="B131" s="57"/>
-      <c r="C131" s="57"/>
-      <c r="D131" s="57"/>
-      <c r="E131" s="57"/>
-      <c r="F131" s="57"/>
-      <c r="G131" s="57"/>
-      <c r="H131" s="57"/>
-      <c r="I131" s="57"/>
-      <c r="J131" s="57"/>
-      <c r="K131" s="57"/>
-      <c r="L131" s="57"/>
+      <c r="B131" s="50"/>
+      <c r="C131" s="50"/>
+      <c r="D131" s="50"/>
+      <c r="E131" s="50"/>
+      <c r="F131" s="50"/>
+      <c r="G131" s="50"/>
+      <c r="H131" s="50"/>
+      <c r="I131" s="50"/>
+      <c r="J131" s="50"/>
+      <c r="K131" s="50"/>
+      <c r="L131" s="50"/>
     </row>
     <row r="132" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A132" s="46" t="s">
+      <c r="A132" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="B132" s="46"/>
-      <c r="C132" s="46"/>
-      <c r="D132" s="46"/>
-      <c r="E132" s="46"/>
-      <c r="F132" s="47"/>
+      <c r="B132" s="51"/>
+      <c r="C132" s="51"/>
+      <c r="D132" s="51"/>
+      <c r="E132" s="51"/>
+      <c r="F132" s="52"/>
     </row>
     <row r="133" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A133" s="48" t="s">
+      <c r="A133" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B133" s="49"/>
+      <c r="B133" s="54"/>
       <c r="C133" s="21">
         <v>7</v>
       </c>
-      <c r="D133" s="50" t="s">
+      <c r="D133" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E133" s="51"/>
-      <c r="F133" s="52"/>
+      <c r="E133" s="56"/>
+      <c r="F133" s="57"/>
     </row>
     <row r="134" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="42" t="s">
@@ -4618,7 +4936,7 @@
         <v>11</v>
       </c>
       <c r="C136" s="31">
-        <f t="shared" ref="C136:C139" si="42">((B136-A136+1)*0.05)</f>
+        <f t="shared" ref="C136:C139" si="48">((B136-A136+1)*0.05)</f>
         <v>0.15000000000000002</v>
       </c>
       <c r="D136" s="18">
@@ -4628,20 +4946,20 @@
         <v>50</v>
       </c>
       <c r="F136" s="19">
-        <f t="shared" ref="F136:F139" si="43">D136*E136</f>
+        <f t="shared" ref="F136:F139" si="49">D136*E136</f>
         <v>150</v>
       </c>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="43">
-        <f t="shared" ref="A137:A139" si="44">B136+1</f>
+        <f t="shared" ref="A137:A139" si="50">B136+1</f>
         <v>12</v>
       </c>
       <c r="B137" s="8">
         <v>18</v>
       </c>
       <c r="C137" s="31">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>0.35000000000000003</v>
       </c>
       <c r="D137" s="18">
@@ -4651,20 +4969,20 @@
         <v>100</v>
       </c>
       <c r="F137" s="19">
-        <f t="shared" si="43"/>
+        <f t="shared" si="49"/>
         <v>200</v>
       </c>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="43">
-        <f t="shared" si="44"/>
+        <f t="shared" si="50"/>
         <v>19</v>
       </c>
       <c r="B138" s="8">
         <v>23</v>
       </c>
       <c r="C138" s="31">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>0.25</v>
       </c>
       <c r="D138" s="18">
@@ -4674,13 +4992,13 @@
         <v>200</v>
       </c>
       <c r="F138" s="19">
-        <f t="shared" si="43"/>
+        <f t="shared" si="49"/>
         <v>400</v>
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="43">
-        <f t="shared" si="44"/>
+        <f t="shared" si="50"/>
         <v>24</v>
       </c>
       <c r="B139" s="44">
@@ -4688,7 +5006,7 @@
         <v>27</v>
       </c>
       <c r="C139" s="31">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>0.2</v>
       </c>
       <c r="D139" s="20">
@@ -4698,67 +5016,67 @@
         <v>200</v>
       </c>
       <c r="F139" s="22">
-        <f t="shared" si="43"/>
+        <f t="shared" si="49"/>
         <v>600</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A140" s="53" t="s">
+      <c r="A140" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B140" s="54"/>
+      <c r="B140" s="47"/>
       <c r="C140" s="33">
         <f>'Individual Treasure'!B16</f>
         <v>318.40814976470659</v>
       </c>
-      <c r="D140" s="55" t="s">
+      <c r="D140" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E140" s="56"/>
+      <c r="E140" s="49"/>
       <c r="F140" s="34">
         <f>SUMPRODUCT(C135:C139,F135:F139)</f>
         <v>317.5</v>
       </c>
     </row>
     <row r="141" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A141" s="57" t="s">
+      <c r="A141" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="B141" s="57"/>
-      <c r="C141" s="57"/>
-      <c r="D141" s="57"/>
-      <c r="E141" s="57"/>
-      <c r="F141" s="57"/>
-      <c r="G141" s="57"/>
-      <c r="H141" s="57"/>
-      <c r="I141" s="57"/>
-      <c r="J141" s="57"/>
-      <c r="K141" s="57"/>
-      <c r="L141" s="57"/>
+      <c r="B141" s="50"/>
+      <c r="C141" s="50"/>
+      <c r="D141" s="50"/>
+      <c r="E141" s="50"/>
+      <c r="F141" s="50"/>
+      <c r="G141" s="50"/>
+      <c r="H141" s="50"/>
+      <c r="I141" s="50"/>
+      <c r="J141" s="50"/>
+      <c r="K141" s="50"/>
+      <c r="L141" s="50"/>
     </row>
     <row r="142" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A142" s="46" t="s">
+      <c r="A142" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="B142" s="46"/>
-      <c r="C142" s="46"/>
-      <c r="D142" s="46"/>
-      <c r="E142" s="46"/>
-      <c r="F142" s="47"/>
-    </row>
-    <row r="143" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A143" s="48" t="s">
+      <c r="B142" s="51"/>
+      <c r="C142" s="51"/>
+      <c r="D142" s="51"/>
+      <c r="E142" s="51"/>
+      <c r="F142" s="52"/>
+    </row>
+    <row r="143" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B143" s="49"/>
+      <c r="B143" s="54"/>
       <c r="C143" s="21">
         <v>7</v>
       </c>
-      <c r="D143" s="50" t="s">
+      <c r="D143" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E143" s="51"/>
-      <c r="F143" s="52"/>
+      <c r="E143" s="56"/>
+      <c r="F143" s="57"/>
     </row>
     <row r="144" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="42" t="s">
@@ -4812,7 +5130,7 @@
         <v>14</v>
       </c>
       <c r="C146" s="31">
-        <f t="shared" ref="C146:C149" si="45">((B146-A146+1)*0.05)</f>
+        <f t="shared" ref="C146:C149" si="51">((B146-A146+1)*0.05)</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="D146" s="18">
@@ -4822,20 +5140,20 @@
         <v>100</v>
       </c>
       <c r="F146" s="19">
-        <f t="shared" ref="F146:F149" si="46">D146*E146</f>
+        <f t="shared" ref="F146:F149" si="52">D146*E146</f>
         <v>300</v>
       </c>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="43">
-        <f t="shared" ref="A147:A149" si="47">B146+1</f>
+        <f t="shared" ref="A147:A149" si="53">B146+1</f>
         <v>15</v>
       </c>
       <c r="B147" s="8">
         <v>19</v>
       </c>
       <c r="C147" s="31">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0.25</v>
       </c>
       <c r="D147" s="18">
@@ -4845,20 +5163,20 @@
         <v>200</v>
       </c>
       <c r="F147" s="19">
-        <f t="shared" si="46"/>
+        <f t="shared" si="52"/>
         <v>400</v>
       </c>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="43">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>20</v>
       </c>
       <c r="B148" s="8">
         <v>23</v>
       </c>
       <c r="C148" s="31">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0.2</v>
       </c>
       <c r="D148" s="18">
@@ -4868,13 +5186,13 @@
         <v>500</v>
       </c>
       <c r="F148" s="19">
-        <f t="shared" si="46"/>
+        <f t="shared" si="52"/>
         <v>500</v>
       </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="43">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>24</v>
       </c>
       <c r="B149" s="44">
@@ -4882,7 +5200,7 @@
         <v>27</v>
       </c>
       <c r="C149" s="31">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0.2</v>
       </c>
       <c r="D149" s="20">
@@ -4892,67 +5210,67 @@
         <v>1000</v>
       </c>
       <c r="F149" s="22">
-        <f t="shared" si="46"/>
+        <f t="shared" si="52"/>
         <v>1000</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A150" s="53" t="s">
+    <row r="150" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B150" s="54"/>
+      <c r="B150" s="47"/>
       <c r="C150" s="33">
         <f>'Individual Treasure'!B17</f>
         <v>493.13849111663814</v>
       </c>
-      <c r="D150" s="55" t="s">
+      <c r="D150" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E150" s="56"/>
+      <c r="E150" s="49"/>
       <c r="F150" s="34">
         <f>SUMPRODUCT(C145:C149,F145:F149)</f>
         <v>495</v>
       </c>
     </row>
     <row r="151" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A151" s="57" t="s">
+      <c r="A151" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="B151" s="57"/>
-      <c r="C151" s="57"/>
-      <c r="D151" s="57"/>
-      <c r="E151" s="57"/>
-      <c r="F151" s="57"/>
-      <c r="G151" s="57"/>
-      <c r="H151" s="57"/>
-      <c r="I151" s="57"/>
-      <c r="J151" s="57"/>
-      <c r="K151" s="57"/>
-      <c r="L151" s="57"/>
+      <c r="B151" s="50"/>
+      <c r="C151" s="50"/>
+      <c r="D151" s="50"/>
+      <c r="E151" s="50"/>
+      <c r="F151" s="50"/>
+      <c r="G151" s="50"/>
+      <c r="H151" s="50"/>
+      <c r="I151" s="50"/>
+      <c r="J151" s="50"/>
+      <c r="K151" s="50"/>
+      <c r="L151" s="50"/>
     </row>
     <row r="152" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A152" s="46" t="s">
+      <c r="A152" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="B152" s="46"/>
-      <c r="C152" s="46"/>
-      <c r="D152" s="46"/>
-      <c r="E152" s="46"/>
-      <c r="F152" s="47"/>
+      <c r="B152" s="51"/>
+      <c r="C152" s="51"/>
+      <c r="D152" s="51"/>
+      <c r="E152" s="51"/>
+      <c r="F152" s="52"/>
     </row>
     <row r="153" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A153" s="48" t="s">
+      <c r="A153" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B153" s="49"/>
+      <c r="B153" s="54"/>
       <c r="C153" s="21">
         <v>7</v>
       </c>
-      <c r="D153" s="50" t="s">
+      <c r="D153" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E153" s="51"/>
-      <c r="F153" s="52"/>
+      <c r="E153" s="56"/>
+      <c r="F153" s="57"/>
     </row>
     <row r="154" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="42" t="s">
@@ -5006,7 +5324,7 @@
         <v>13</v>
       </c>
       <c r="C156" s="31">
-        <f t="shared" ref="C156:C159" si="48">((B156-A156+1)*0.05)</f>
+        <f t="shared" ref="C156:C159" si="54">((B156-A156+1)*0.05)</f>
         <v>0.25</v>
       </c>
       <c r="D156" s="18">
@@ -5016,20 +5334,20 @@
         <v>100</v>
       </c>
       <c r="F156" s="19">
-        <f t="shared" ref="F156:F159" si="49">D156*E156</f>
+        <f t="shared" ref="F156:F159" si="55">D156*E156</f>
         <v>300</v>
       </c>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="43">
-        <f t="shared" ref="A157:A159" si="50">B156+1</f>
+        <f t="shared" ref="A157:A159" si="56">B156+1</f>
         <v>14</v>
       </c>
       <c r="B157" s="8">
         <v>18</v>
       </c>
       <c r="C157" s="31">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.25</v>
       </c>
       <c r="D157" s="18">
@@ -5039,20 +5357,20 @@
         <v>500</v>
       </c>
       <c r="F157" s="19">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>500</v>
       </c>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="43">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>19</v>
       </c>
       <c r="B158" s="8">
         <v>25</v>
       </c>
       <c r="C158" s="31">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.35000000000000003</v>
       </c>
       <c r="D158" s="18">
@@ -5062,13 +5380,13 @@
         <v>1000</v>
       </c>
       <c r="F158" s="19">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>1000</v>
       </c>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="43">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>26</v>
       </c>
       <c r="B159" s="44">
@@ -5076,7 +5394,7 @@
         <v>27</v>
       </c>
       <c r="C159" s="31">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.1</v>
       </c>
       <c r="D159" s="20">
@@ -5086,67 +5404,67 @@
         <v>1000</v>
       </c>
       <c r="F159" s="22">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>2000</v>
       </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A160" s="53" t="s">
+      <c r="A160" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B160" s="54"/>
+      <c r="B160" s="47"/>
       <c r="C160" s="33">
         <f>'Individual Treasure'!B18</f>
         <v>763.75423053869986</v>
       </c>
-      <c r="D160" s="55" t="s">
+      <c r="D160" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E160" s="56"/>
+      <c r="E160" s="49"/>
       <c r="F160" s="34">
         <f>SUMPRODUCT(C155:C159,F155:F159)</f>
         <v>760</v>
       </c>
     </row>
     <row r="161" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A161" s="57" t="s">
+      <c r="A161" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="B161" s="57"/>
-      <c r="C161" s="57"/>
-      <c r="D161" s="57"/>
-      <c r="E161" s="57"/>
-      <c r="F161" s="57"/>
-      <c r="G161" s="57"/>
-      <c r="H161" s="57"/>
-      <c r="I161" s="57"/>
-      <c r="J161" s="57"/>
-      <c r="K161" s="57"/>
-      <c r="L161" s="57"/>
+      <c r="B161" s="50"/>
+      <c r="C161" s="50"/>
+      <c r="D161" s="50"/>
+      <c r="E161" s="50"/>
+      <c r="F161" s="50"/>
+      <c r="G161" s="50"/>
+      <c r="H161" s="50"/>
+      <c r="I161" s="50"/>
+      <c r="J161" s="50"/>
+      <c r="K161" s="50"/>
+      <c r="L161" s="50"/>
     </row>
     <row r="162" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A162" s="46" t="s">
+      <c r="A162" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="B162" s="46"/>
-      <c r="C162" s="46"/>
-      <c r="D162" s="46"/>
-      <c r="E162" s="46"/>
-      <c r="F162" s="47"/>
+      <c r="B162" s="51"/>
+      <c r="C162" s="51"/>
+      <c r="D162" s="51"/>
+      <c r="E162" s="51"/>
+      <c r="F162" s="52"/>
     </row>
     <row r="163" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A163" s="48" t="s">
+      <c r="A163" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B163" s="49"/>
+      <c r="B163" s="54"/>
       <c r="C163" s="21">
         <v>7</v>
       </c>
-      <c r="D163" s="50" t="s">
+      <c r="D163" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E163" s="51"/>
-      <c r="F163" s="52"/>
+      <c r="E163" s="56"/>
+      <c r="F163" s="57"/>
     </row>
     <row r="164" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="42" t="s">
@@ -5200,7 +5518,7 @@
         <v>14</v>
       </c>
       <c r="C166" s="31">
-        <f t="shared" ref="C166:C169" si="51">((B166-A166+1)*0.05)</f>
+        <f t="shared" ref="C166:C169" si="57">((B166-A166+1)*0.05)</f>
         <v>0.25</v>
       </c>
       <c r="D166" s="18">
@@ -5210,20 +5528,20 @@
         <v>500</v>
       </c>
       <c r="F166" s="19">
-        <f t="shared" ref="F166:F169" si="52">D166*E166</f>
+        <f t="shared" ref="F166:F169" si="58">D166*E166</f>
         <v>500</v>
       </c>
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" s="43">
-        <f t="shared" ref="A167:A169" si="53">B166+1</f>
+        <f t="shared" ref="A167:A169" si="59">B166+1</f>
         <v>15</v>
       </c>
       <c r="B167" s="8">
         <v>20</v>
       </c>
       <c r="C167" s="31">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="D167" s="18">
@@ -5233,20 +5551,20 @@
         <v>500</v>
       </c>
       <c r="F167" s="19">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1000</v>
       </c>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" s="43">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>21</v>
       </c>
       <c r="B168" s="8">
         <v>26</v>
       </c>
       <c r="C168" s="31">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="D168" s="18">
@@ -5256,13 +5574,13 @@
         <v>1000</v>
       </c>
       <c r="F168" s="19">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>2000</v>
       </c>
     </row>
     <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" s="43">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>27</v>
       </c>
       <c r="B169" s="44">
@@ -5270,7 +5588,7 @@
         <v>27</v>
       </c>
       <c r="C169" s="31">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>0.05</v>
       </c>
       <c r="D169" s="20">
@@ -5280,69 +5598,89 @@
         <v>1000</v>
       </c>
       <c r="F169" s="22">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>3000</v>
       </c>
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A170" s="53" t="s">
+      <c r="A170" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B170" s="54"/>
+      <c r="B170" s="47"/>
       <c r="C170" s="33">
         <f>'Individual Treasure'!B19</f>
         <v>1182.8736453829017</v>
       </c>
-      <c r="D170" s="55" t="s">
+      <c r="D170" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E170" s="56"/>
+      <c r="E170" s="49"/>
       <c r="F170" s="34">
         <f>SUMPRODUCT(C165:C169,F165:F169)</f>
         <v>1205.0000000000002</v>
       </c>
     </row>
     <row r="171" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A171" s="57" t="s">
+      <c r="A171" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="B171" s="57"/>
-      <c r="C171" s="57"/>
-      <c r="D171" s="57"/>
-      <c r="E171" s="57"/>
-      <c r="F171" s="57"/>
-      <c r="G171" s="57"/>
-      <c r="H171" s="57"/>
-      <c r="I171" s="57"/>
-      <c r="J171" s="57"/>
-      <c r="K171" s="57"/>
-      <c r="L171" s="57"/>
+      <c r="B171" s="50"/>
+      <c r="C171" s="50"/>
+      <c r="D171" s="50"/>
+      <c r="E171" s="50"/>
+      <c r="F171" s="50"/>
+      <c r="G171" s="50"/>
+      <c r="H171" s="50"/>
+      <c r="I171" s="50"/>
+      <c r="J171" s="50"/>
+      <c r="K171" s="50"/>
+      <c r="L171" s="50"/>
     </row>
     <row r="172" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A172" s="46" t="s">
+      <c r="A172" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="B172" s="46"/>
-      <c r="C172" s="46"/>
-      <c r="D172" s="46"/>
-      <c r="E172" s="46"/>
-      <c r="F172" s="47"/>
-    </row>
-    <row r="173" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A173" s="48" t="s">
+      <c r="B172" s="51"/>
+      <c r="C172" s="51"/>
+      <c r="D172" s="51"/>
+      <c r="E172" s="51"/>
+      <c r="F172" s="52"/>
+      <c r="G172" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="H172" s="51"/>
+      <c r="I172" s="51"/>
+      <c r="J172" s="51"/>
+      <c r="K172" s="51"/>
+      <c r="L172" s="52"/>
+    </row>
+    <row r="173" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B173" s="49"/>
+      <c r="B173" s="54"/>
       <c r="C173" s="21">
         <v>7</v>
       </c>
-      <c r="D173" s="50" t="s">
+      <c r="D173" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E173" s="51"/>
-      <c r="F173" s="52"/>
-    </row>
-    <row r="174" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="E173" s="56"/>
+      <c r="F173" s="57"/>
+      <c r="G173" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="H173" s="54"/>
+      <c r="I173" s="21">
+        <v>7</v>
+      </c>
+      <c r="J173" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="K173" s="56"/>
+      <c r="L173" s="57"/>
+    </row>
+    <row r="174" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A174" s="42" t="s">
         <v>9</v>
       </c>
@@ -5359,6 +5697,24 @@
         <v>24</v>
       </c>
       <c r="F174" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G174" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H174" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I174" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="J174" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="K174" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="L174" s="17" t="s">
         <v>44</v>
       </c>
     </row>
@@ -5384,6 +5740,27 @@
         <f>D175*E175</f>
         <v>500</v>
       </c>
+      <c r="G175" s="43">
+        <f>I173+1</f>
+        <v>8</v>
+      </c>
+      <c r="H175" s="8">
+        <v>9</v>
+      </c>
+      <c r="I175" s="31">
+        <f>((H175-G175+1)*0.05)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J175" s="18">
+        <v>1</v>
+      </c>
+      <c r="K175" s="8">
+        <v>500</v>
+      </c>
+      <c r="L175" s="19">
+        <f>J175*K175</f>
+        <v>500</v>
+      </c>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A176" s="43">
@@ -5394,7 +5771,7 @@
         <v>12</v>
       </c>
       <c r="C176" s="31">
-        <f t="shared" ref="C176:C179" si="54">((B176-A176+1)*0.05)</f>
+        <f t="shared" ref="C176:C179" si="60">((B176-A176+1)*0.05)</f>
         <v>0.15000000000000002</v>
       </c>
       <c r="D176" s="18">
@@ -5404,20 +5781,41 @@
         <v>500</v>
       </c>
       <c r="F176" s="19">
-        <f t="shared" ref="F176:F179" si="55">D176*E176</f>
+        <f t="shared" ref="F176:F179" si="61">D176*E176</f>
+        <v>1000</v>
+      </c>
+      <c r="G176" s="43">
+        <f>H175+1</f>
+        <v>10</v>
+      </c>
+      <c r="H176" s="8">
+        <v>12</v>
+      </c>
+      <c r="I176" s="31">
+        <f t="shared" ref="I176:I179" si="62">((H176-G176+1)*0.05)</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="J176" s="18">
+        <v>2</v>
+      </c>
+      <c r="K176" s="8">
+        <v>500</v>
+      </c>
+      <c r="L176" s="19">
+        <f t="shared" ref="L176:L179" si="63">J176*K176</f>
         <v>1000</v>
       </c>
     </row>
     <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177" s="43">
-        <f t="shared" ref="A177:A179" si="56">B176+1</f>
+        <f t="shared" ref="A177:A179" si="64">B176+1</f>
         <v>13</v>
       </c>
       <c r="B177" s="8">
         <v>18</v>
       </c>
       <c r="C177" s="31">
-        <f t="shared" si="54"/>
+        <f t="shared" si="60"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="D177" s="18">
@@ -5427,20 +5825,41 @@
         <v>500</v>
       </c>
       <c r="F177" s="19">
-        <f t="shared" si="55"/>
+        <f t="shared" si="61"/>
+        <v>1500</v>
+      </c>
+      <c r="G177" s="43">
+        <f t="shared" ref="G177:G179" si="65">H176+1</f>
+        <v>13</v>
+      </c>
+      <c r="H177" s="8">
+        <v>18</v>
+      </c>
+      <c r="I177" s="31">
+        <f t="shared" si="62"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="J177" s="18">
+        <v>3</v>
+      </c>
+      <c r="K177" s="8">
+        <v>500</v>
+      </c>
+      <c r="L177" s="19">
+        <f t="shared" si="63"/>
         <v>1500</v>
       </c>
     </row>
     <row r="178" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A178" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="64"/>
         <v>19</v>
       </c>
       <c r="B178" s="8">
         <v>24</v>
       </c>
       <c r="C178" s="31">
-        <f t="shared" si="54"/>
+        <f t="shared" si="60"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="D178" s="18">
@@ -5450,13 +5869,34 @@
         <v>1000</v>
       </c>
       <c r="F178" s="19">
-        <f t="shared" si="55"/>
+        <f t="shared" si="61"/>
+        <v>2000</v>
+      </c>
+      <c r="G178" s="43">
+        <f t="shared" si="65"/>
+        <v>19</v>
+      </c>
+      <c r="H178" s="8">
+        <v>24</v>
+      </c>
+      <c r="I178" s="31">
+        <f t="shared" si="62"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="J178" s="18">
+        <v>2</v>
+      </c>
+      <c r="K178" s="8">
+        <v>1000</v>
+      </c>
+      <c r="L178" s="19">
+        <f t="shared" si="63"/>
         <v>2000</v>
       </c>
     </row>
     <row r="179" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A179" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="64"/>
         <v>25</v>
       </c>
       <c r="B179" s="44">
@@ -5464,7 +5904,7 @@
         <v>27</v>
       </c>
       <c r="C179" s="31">
-        <f t="shared" si="54"/>
+        <f t="shared" si="60"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="D179" s="20">
@@ -5474,67 +5914,105 @@
         <v>2000</v>
       </c>
       <c r="F179" s="22">
-        <f t="shared" si="55"/>
+        <f t="shared" si="61"/>
         <v>4000</v>
       </c>
-    </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A180" s="53" t="s">
+      <c r="G179" s="43">
+        <f t="shared" si="65"/>
+        <v>25</v>
+      </c>
+      <c r="H179" s="44">
+        <f>20+I173</f>
+        <v>27</v>
+      </c>
+      <c r="I179" s="31">
+        <f t="shared" si="62"/>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="J179" s="20">
+        <v>2</v>
+      </c>
+      <c r="K179" s="28">
+        <v>2000</v>
+      </c>
+      <c r="L179" s="22">
+        <f t="shared" si="63"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B180" s="54"/>
+      <c r="B180" s="47"/>
       <c r="C180" s="33">
         <f>'Individual Treasure'!B20</f>
         <v>1831.989932094441</v>
       </c>
-      <c r="D180" s="55" t="s">
+      <c r="D180" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E180" s="56"/>
+      <c r="E180" s="49"/>
       <c r="F180" s="34">
         <f>SUMPRODUCT(C175:C179,F175:F179)</f>
         <v>1850.0000000000005</v>
       </c>
+      <c r="G180" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="H180" s="47"/>
+      <c r="I180" s="33">
+        <f>'Individual Treasure'!H20</f>
+        <v>0</v>
+      </c>
+      <c r="J180" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="K180" s="49"/>
+      <c r="L180" s="34">
+        <f>SUMPRODUCT(I175:I179,L175:L179)</f>
+        <v>1850.0000000000005</v>
+      </c>
     </row>
     <row r="181" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A181" s="57" t="s">
+      <c r="A181" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="B181" s="57"/>
-      <c r="C181" s="57"/>
-      <c r="D181" s="57"/>
-      <c r="E181" s="57"/>
-      <c r="F181" s="57"/>
-      <c r="G181" s="57"/>
-      <c r="H181" s="57"/>
-      <c r="I181" s="57"/>
-      <c r="J181" s="57"/>
-      <c r="K181" s="57"/>
-      <c r="L181" s="57"/>
+      <c r="B181" s="50"/>
+      <c r="C181" s="50"/>
+      <c r="D181" s="50"/>
+      <c r="E181" s="50"/>
+      <c r="F181" s="50"/>
+      <c r="G181" s="50"/>
+      <c r="H181" s="50"/>
+      <c r="I181" s="50"/>
+      <c r="J181" s="50"/>
+      <c r="K181" s="50"/>
+      <c r="L181" s="50"/>
     </row>
     <row r="182" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A182" s="46" t="s">
+      <c r="A182" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="B182" s="46"/>
-      <c r="C182" s="46"/>
-      <c r="D182" s="46"/>
-      <c r="E182" s="46"/>
-      <c r="F182" s="47"/>
+      <c r="B182" s="51"/>
+      <c r="C182" s="51"/>
+      <c r="D182" s="51"/>
+      <c r="E182" s="51"/>
+      <c r="F182" s="52"/>
     </row>
     <row r="183" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A183" s="48" t="s">
+      <c r="A183" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B183" s="49"/>
+      <c r="B183" s="54"/>
       <c r="C183" s="21">
         <v>7</v>
       </c>
-      <c r="D183" s="50" t="s">
+      <c r="D183" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="E183" s="51"/>
-      <c r="F183" s="52"/>
+      <c r="E183" s="56"/>
+      <c r="F183" s="57"/>
     </row>
     <row r="184" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="42" t="s">
@@ -5588,7 +6066,7 @@
         <v>11</v>
       </c>
       <c r="C186" s="31">
-        <f t="shared" ref="C186:C189" si="57">((B186-A186+1)*0.05)</f>
+        <f t="shared" ref="C186:C189" si="66">((B186-A186+1)*0.05)</f>
         <v>0.1</v>
       </c>
       <c r="D186" s="18">
@@ -5598,20 +6076,20 @@
         <v>1000</v>
       </c>
       <c r="F186" s="19">
-        <f t="shared" ref="F186:F189" si="58">D186*E186</f>
+        <f t="shared" ref="F186:F189" si="67">D186*E186</f>
         <v>1000</v>
       </c>
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187" s="43">
-        <f t="shared" ref="A187:A189" si="59">B186+1</f>
+        <f t="shared" ref="A187:A189" si="68">B186+1</f>
         <v>12</v>
       </c>
       <c r="B187" s="8">
         <v>17</v>
       </c>
       <c r="C187" s="31">
-        <f t="shared" si="57"/>
+        <f t="shared" si="66"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="D187" s="18">
@@ -5621,20 +6099,20 @@
         <v>1000</v>
       </c>
       <c r="F187" s="19">
-        <f t="shared" si="58"/>
+        <f t="shared" si="67"/>
         <v>2000</v>
       </c>
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="68"/>
         <v>18</v>
       </c>
       <c r="B188" s="8">
         <v>23</v>
       </c>
       <c r="C188" s="31">
-        <f t="shared" si="57"/>
+        <f t="shared" si="66"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="D188" s="18">
@@ -5644,13 +6122,13 @@
         <v>1000</v>
       </c>
       <c r="F188" s="19">
-        <f t="shared" si="58"/>
+        <f t="shared" si="67"/>
         <v>3000</v>
       </c>
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="68"/>
         <v>24</v>
       </c>
       <c r="B189" s="44">
@@ -5658,7 +6136,7 @@
         <v>27</v>
       </c>
       <c r="C189" s="31">
-        <f t="shared" si="57"/>
+        <f t="shared" si="66"/>
         <v>0.2</v>
       </c>
       <c r="D189" s="20">
@@ -5668,120 +6146,40 @@
         <v>2000</v>
       </c>
       <c r="F189" s="22">
-        <f t="shared" si="58"/>
+        <f t="shared" si="67"/>
         <v>6000</v>
       </c>
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A190" s="53" t="s">
+      <c r="A190" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B190" s="54"/>
+      <c r="B190" s="47"/>
       <c r="C190" s="33">
         <f>'Individual Treasure'!B21</f>
         <v>2837.3166689405625</v>
       </c>
-      <c r="D190" s="55" t="s">
+      <c r="D190" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E190" s="56"/>
+      <c r="E190" s="49"/>
       <c r="F190" s="34">
         <f>SUMPRODUCT(C185:C189,F185:F189)</f>
         <v>2850</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="119">
-    <mergeCell ref="A180:B180"/>
-    <mergeCell ref="D180:E180"/>
-    <mergeCell ref="A181:L181"/>
-    <mergeCell ref="A182:F182"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="D183:F183"/>
-    <mergeCell ref="A190:B190"/>
-    <mergeCell ref="D190:E190"/>
-    <mergeCell ref="A161:L161"/>
-    <mergeCell ref="A162:F162"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="D163:F163"/>
-    <mergeCell ref="A170:B170"/>
-    <mergeCell ref="D170:E170"/>
-    <mergeCell ref="A171:L171"/>
-    <mergeCell ref="A172:F172"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="D173:F173"/>
-    <mergeCell ref="A151:L151"/>
-    <mergeCell ref="A152:F152"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="D153:F153"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="D160:E160"/>
-    <mergeCell ref="A141:L141"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="D143:F143"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="D150:E150"/>
-    <mergeCell ref="A131:L131"/>
-    <mergeCell ref="A132:F132"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="D133:F133"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="D140:E140"/>
-    <mergeCell ref="A121:L121"/>
-    <mergeCell ref="A122:F122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D123:F123"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="A111:L111"/>
-    <mergeCell ref="A112:F112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D113:F113"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D120:E120"/>
-    <mergeCell ref="A101:L101"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D103:F103"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="A91:L91"/>
-    <mergeCell ref="A92:F92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:F93"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="A81:L81"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="A71:L71"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="A61:L61"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="A51:L51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="A41:L41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
+  <mergeCells count="134">
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="A31:L31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="G92:L92"/>
+    <mergeCell ref="G93:H93"/>
+    <mergeCell ref="J93:L93"/>
+    <mergeCell ref="G100:H100"/>
+    <mergeCell ref="J100:K100"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="D20:E20"/>
@@ -5806,11 +6204,106 @@
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="J23:L23"/>
     <mergeCell ref="G30:H30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="A31:L31"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="A51:L51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A41:L41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="A71:L71"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="A61:L61"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="A91:L91"/>
+    <mergeCell ref="A92:F92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:F93"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="A81:L81"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="A111:L111"/>
+    <mergeCell ref="A112:F112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D113:F113"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="A101:L101"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D103:F103"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="A131:L131"/>
+    <mergeCell ref="A132:F132"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="D133:F133"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="D140:E140"/>
+    <mergeCell ref="A121:L121"/>
+    <mergeCell ref="A122:F122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D123:F123"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="G122:L122"/>
+    <mergeCell ref="G123:H123"/>
+    <mergeCell ref="J123:L123"/>
+    <mergeCell ref="G130:H130"/>
+    <mergeCell ref="J130:K130"/>
+    <mergeCell ref="A151:L151"/>
+    <mergeCell ref="A152:F152"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="D153:F153"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="D160:E160"/>
+    <mergeCell ref="A141:L141"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="D143:F143"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="D180:E180"/>
+    <mergeCell ref="A181:L181"/>
+    <mergeCell ref="A182:F182"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="D183:F183"/>
+    <mergeCell ref="A190:B190"/>
+    <mergeCell ref="D190:E190"/>
+    <mergeCell ref="A161:L161"/>
+    <mergeCell ref="A162:F162"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="D163:F163"/>
+    <mergeCell ref="A170:B170"/>
+    <mergeCell ref="D170:E170"/>
+    <mergeCell ref="A171:L171"/>
+    <mergeCell ref="A172:F172"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="D173:F173"/>
+    <mergeCell ref="G172:L172"/>
+    <mergeCell ref="G173:H173"/>
+    <mergeCell ref="J173:L173"/>
+    <mergeCell ref="G180:H180"/>
+    <mergeCell ref="J180:K180"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5881,7 +6374,7 @@
       <c r="W1" s="63"/>
     </row>
     <row r="2" spans="1:23" s="14" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="53" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="64"/>
@@ -6800,7 +7293,7 @@
       <c r="W1" s="63"/>
     </row>
     <row r="2" spans="1:23" s="14" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="53" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="64"/>
@@ -7719,7 +8212,7 @@
       <c r="W1" s="63"/>
     </row>
     <row r="2" spans="1:23" s="14" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="53" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="64"/>

</xml_diff>

<commit_message>
Add severl high level treasure averages
</commit_message>
<xml_diff>
--- a/Individual Treasure Averages.xlsx
+++ b/Individual Treasure Averages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD63BF2-B39B-440B-BF2F-D5782B389F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405FF609-75E4-4345-A359-D03A0496D57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="616" activeTab="1" xr2:uid="{5E3698F5-01A8-41EE-A738-BAB99CC962C2}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="95">
   <si>
     <t>Individual gp Per Formula</t>
   </si>
@@ -294,6 +294,27 @@
   </si>
   <si>
     <t>CR 10: Large Creature</t>
+  </si>
+  <si>
+    <t>CR 17 Individual Treasure Tables</t>
+  </si>
+  <si>
+    <t>CR 17: Humanoid</t>
+  </si>
+  <si>
+    <t>CR 20 Individual Treasure Tables</t>
+  </si>
+  <si>
+    <t>CR 20: Humanoid</t>
+  </si>
+  <si>
+    <t>CR 22 Individual Treasure Tables</t>
+  </si>
+  <si>
+    <t>CR 22: Humanoid</t>
+  </si>
+  <si>
+    <t>CR 24 Individual Treasure Tables</t>
   </si>
 </sst>
 </file>
@@ -673,12 +694,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -708,6 +723,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -723,6 +744,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -731,9 +755,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1052,7 +1073,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,10 +1677,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD8D082-213D-4692-B6C5-868C3C1BDB24}">
-  <dimension ref="A1:AD190"/>
+  <dimension ref="A1:AD230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
+      <selection activeCell="G230" sqref="G230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,20 +1719,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
       <c r="Z1" s="39"/>
       <c r="AA1" s="39"/>
       <c r="AB1" s="39"/>
@@ -1753,10 +1774,10 @@
       <c r="AD2" s="37"/>
     </row>
     <row r="3" spans="1:30" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="54"/>
+      <c r="B3" s="52"/>
       <c r="C3" s="21">
         <v>3</v>
       </c>
@@ -1951,18 +1972,18 @@
       </c>
     </row>
     <row r="10" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="47"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="33">
         <f>'Individual Treasure'!B3</f>
         <v>1.0794007754789445</v>
       </c>
-      <c r="D10" s="48" t="s">
+      <c r="D10" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="49"/>
+      <c r="E10" s="47"/>
       <c r="F10" s="34">
         <f>SUMPRODUCT(C5:C9,F5:F9)</f>
         <v>1</v>
@@ -1988,20 +2009,20 @@
       <c r="AD10" s="13"/>
     </row>
     <row r="11" spans="1:30" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
       <c r="Z11" s="39"/>
       <c r="AA11" s="39"/>
       <c r="AB11" s="39"/>
@@ -2009,14 +2030,14 @@
       <c r="AD11" s="39"/>
     </row>
     <row r="12" spans="1:30" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="52"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="50"/>
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
       <c r="I12" s="37"/>
@@ -2043,18 +2064,18 @@
       <c r="AD12" s="37"/>
     </row>
     <row r="13" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="54"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="21">
         <v>3</v>
       </c>
-      <c r="D13" s="55" t="s">
+      <c r="D13" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="56"/>
-      <c r="F13" s="57"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="55"/>
       <c r="G13" s="38"/>
       <c r="H13" s="38"/>
       <c r="I13" s="36"/>
@@ -2211,18 +2232,18 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="47"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="33">
         <f>'Individual Treasure'!B4</f>
         <v>1.6717350674697367</v>
       </c>
-      <c r="D20" s="48" t="s">
+      <c r="D20" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="49"/>
+      <c r="E20" s="47"/>
       <c r="F20" s="34">
         <f>SUMPRODUCT(C15:C19,F15:F19)</f>
         <v>1.6750000000000003</v>
@@ -2231,64 +2252,64 @@
       <c r="K20" s="13"/>
     </row>
     <row r="21" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
     </row>
     <row r="22" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="51" t="s">
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="H22" s="51"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="51"/>
-      <c r="L22" s="52"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="50"/>
     </row>
     <row r="23" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="54"/>
+      <c r="B23" s="52"/>
       <c r="C23" s="21">
         <v>3</v>
       </c>
-      <c r="D23" s="55" t="s">
+      <c r="D23" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="56"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="53" t="s">
+      <c r="E23" s="54"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="H23" s="54"/>
+      <c r="H23" s="52"/>
       <c r="I23" s="21">
         <v>3</v>
       </c>
-      <c r="J23" s="55" t="s">
+      <c r="J23" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="K23" s="56"/>
-      <c r="L23" s="57"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="55"/>
     </row>
     <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="42" t="s">
@@ -2551,78 +2572,78 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="47"/>
+      <c r="B30" s="57"/>
       <c r="C30" s="33">
         <f>'Individual Treasure'!B5</f>
         <v>2.5891199999999999</v>
       </c>
-      <c r="D30" s="48" t="s">
+      <c r="D30" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="49"/>
+      <c r="E30" s="47"/>
       <c r="F30" s="34">
         <f>SUMPRODUCT(C25:C29,F25:F29)</f>
         <v>2.5750000000000002</v>
       </c>
-      <c r="G30" s="46" t="s">
+      <c r="G30" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="H30" s="47"/>
+      <c r="H30" s="57"/>
       <c r="I30" s="33">
         <f>'Individual Treasure'!B5</f>
         <v>2.5891199999999999</v>
       </c>
-      <c r="J30" s="48" t="s">
+      <c r="J30" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="K30" s="49"/>
+      <c r="K30" s="47"/>
       <c r="L30" s="34">
         <f>SUMPRODUCT(I25:I29,L25:L29)</f>
         <v>2.5499999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="50" t="s">
+      <c r="A31" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="50"/>
-      <c r="L31" s="50"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
     </row>
     <row r="32" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="51"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="52"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="50"/>
     </row>
     <row r="33" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="53" t="s">
+      <c r="A33" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="54"/>
+      <c r="B33" s="52"/>
       <c r="C33" s="21">
         <v>3</v>
       </c>
-      <c r="D33" s="55" t="s">
+      <c r="D33" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E33" s="56"/>
-      <c r="F33" s="57"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="55"/>
     </row>
     <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="42" t="s">
@@ -2761,62 +2782,62 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="46" t="s">
+      <c r="A40" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="47"/>
+      <c r="B40" s="57"/>
       <c r="C40" s="33">
         <f>'Individual Treasure'!B6</f>
         <v>4.0099310619512103</v>
       </c>
-      <c r="D40" s="48" t="s">
+      <c r="D40" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="49"/>
+      <c r="E40" s="47"/>
       <c r="F40" s="34">
         <f>SUMPRODUCT(C35:C39,F35:F39)</f>
         <v>4.05</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="50" t="s">
+      <c r="A41" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="50"/>
-      <c r="I41" s="50"/>
-      <c r="J41" s="50"/>
-      <c r="K41" s="50"/>
-      <c r="L41" s="50"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="48"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="48"/>
+      <c r="K41" s="48"/>
+      <c r="L41" s="48"/>
     </row>
     <row r="42" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A42" s="51" t="s">
+      <c r="A42" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="51"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
-      <c r="F42" s="52"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="50"/>
     </row>
     <row r="43" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="53" t="s">
+      <c r="A43" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="54"/>
+      <c r="B43" s="52"/>
       <c r="C43" s="21">
         <v>3</v>
       </c>
-      <c r="D43" s="55" t="s">
+      <c r="D43" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E43" s="56"/>
-      <c r="F43" s="57"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="55"/>
     </row>
     <row r="44" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="42" t="s">
@@ -2955,62 +2976,62 @@
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="46" t="s">
+      <c r="A50" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="47"/>
+      <c r="B50" s="57"/>
       <c r="C50" s="33">
         <f>'Individual Treasure'!B7</f>
         <v>6.2104294592761873</v>
       </c>
-      <c r="D50" s="48" t="s">
+      <c r="D50" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E50" s="49"/>
+      <c r="E50" s="47"/>
       <c r="F50" s="34">
         <f>SUMPRODUCT(C45:C49,F45:F49)</f>
         <v>6.2000000000000011</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="50" t="s">
+      <c r="A51" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="50"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="50"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="50"/>
-      <c r="H51" s="50"/>
-      <c r="I51" s="50"/>
-      <c r="J51" s="50"/>
-      <c r="K51" s="50"/>
-      <c r="L51" s="50"/>
+      <c r="B51" s="48"/>
+      <c r="C51" s="48"/>
+      <c r="D51" s="48"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="48"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="48"/>
+      <c r="I51" s="48"/>
+      <c r="J51" s="48"/>
+      <c r="K51" s="48"/>
+      <c r="L51" s="48"/>
     </row>
     <row r="52" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A52" s="51" t="s">
+      <c r="A52" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="B52" s="51"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="51"/>
-      <c r="F52" s="52"/>
+      <c r="B52" s="49"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="50"/>
     </row>
     <row r="53" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="53" t="s">
+      <c r="A53" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B53" s="54"/>
+      <c r="B53" s="52"/>
       <c r="C53" s="21">
         <v>3</v>
       </c>
-      <c r="D53" s="55" t="s">
+      <c r="D53" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E53" s="56"/>
-      <c r="F53" s="57"/>
+      <c r="E53" s="54"/>
+      <c r="F53" s="55"/>
     </row>
     <row r="54" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="42" t="s">
@@ -3149,62 +3170,62 @@
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="46" t="s">
+      <c r="A60" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B60" s="47"/>
+      <c r="B60" s="57"/>
       <c r="C60" s="33">
         <f>'Individual Treasure'!B8</f>
         <v>9.6184780917100969</v>
       </c>
-      <c r="D60" s="48" t="s">
+      <c r="D60" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E60" s="49"/>
+      <c r="E60" s="47"/>
       <c r="F60" s="34">
         <f>SUMPRODUCT(C55:C59,F55:F59)</f>
         <v>9.6000000000000014</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="50" t="s">
+      <c r="A61" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="50"/>
-      <c r="C61" s="50"/>
-      <c r="D61" s="50"/>
-      <c r="E61" s="50"/>
-      <c r="F61" s="50"/>
-      <c r="G61" s="50"/>
-      <c r="H61" s="50"/>
-      <c r="I61" s="50"/>
-      <c r="J61" s="50"/>
-      <c r="K61" s="50"/>
-      <c r="L61" s="50"/>
+      <c r="B61" s="48"/>
+      <c r="C61" s="48"/>
+      <c r="D61" s="48"/>
+      <c r="E61" s="48"/>
+      <c r="F61" s="48"/>
+      <c r="G61" s="48"/>
+      <c r="H61" s="48"/>
+      <c r="I61" s="48"/>
+      <c r="J61" s="48"/>
+      <c r="K61" s="48"/>
+      <c r="L61" s="48"/>
     </row>
     <row r="62" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A62" s="51" t="s">
+      <c r="A62" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B62" s="51"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="51"/>
-      <c r="E62" s="51"/>
-      <c r="F62" s="52"/>
+      <c r="B62" s="49"/>
+      <c r="C62" s="49"/>
+      <c r="D62" s="49"/>
+      <c r="E62" s="49"/>
+      <c r="F62" s="50"/>
     </row>
     <row r="63" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="53" t="s">
+      <c r="A63" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B63" s="54"/>
+      <c r="B63" s="52"/>
       <c r="C63" s="21">
         <v>3</v>
       </c>
-      <c r="D63" s="55" t="s">
+      <c r="D63" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E63" s="56"/>
-      <c r="F63" s="57"/>
+      <c r="E63" s="54"/>
+      <c r="F63" s="55"/>
     </row>
     <row r="64" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="42" t="s">
@@ -3343,62 +3364,62 @@
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="46" t="s">
+      <c r="A70" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B70" s="47"/>
+      <c r="B70" s="57"/>
       <c r="C70" s="33">
         <f>'Individual Treasure'!B9</f>
         <v>14.89673482443669</v>
       </c>
-      <c r="D70" s="48" t="s">
+      <c r="D70" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E70" s="49"/>
+      <c r="E70" s="47"/>
       <c r="F70" s="34">
         <f>SUMPRODUCT(C65:C69,F65:F69)</f>
         <v>14.900000000000002</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="50" t="s">
+      <c r="A71" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="B71" s="50"/>
-      <c r="C71" s="50"/>
-      <c r="D71" s="50"/>
-      <c r="E71" s="50"/>
-      <c r="F71" s="50"/>
-      <c r="G71" s="50"/>
-      <c r="H71" s="50"/>
-      <c r="I71" s="50"/>
-      <c r="J71" s="50"/>
-      <c r="K71" s="50"/>
-      <c r="L71" s="50"/>
+      <c r="B71" s="48"/>
+      <c r="C71" s="48"/>
+      <c r="D71" s="48"/>
+      <c r="E71" s="48"/>
+      <c r="F71" s="48"/>
+      <c r="G71" s="48"/>
+      <c r="H71" s="48"/>
+      <c r="I71" s="48"/>
+      <c r="J71" s="48"/>
+      <c r="K71" s="48"/>
+      <c r="L71" s="48"/>
     </row>
     <row r="72" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A72" s="51" t="s">
+      <c r="A72" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B72" s="51"/>
-      <c r="C72" s="51"/>
-      <c r="D72" s="51"/>
-      <c r="E72" s="51"/>
-      <c r="F72" s="52"/>
+      <c r="B72" s="49"/>
+      <c r="C72" s="49"/>
+      <c r="D72" s="49"/>
+      <c r="E72" s="49"/>
+      <c r="F72" s="50"/>
     </row>
     <row r="73" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="53" t="s">
+      <c r="A73" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B73" s="54"/>
+      <c r="B73" s="52"/>
       <c r="C73" s="21">
         <v>5</v>
       </c>
-      <c r="D73" s="55" t="s">
+      <c r="D73" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E73" s="56"/>
-      <c r="F73" s="57"/>
+      <c r="E73" s="54"/>
+      <c r="F73" s="55"/>
     </row>
     <row r="74" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="42" t="s">
@@ -3537,62 +3558,62 @@
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" s="46" t="s">
+      <c r="A80" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B80" s="47"/>
+      <c r="B80" s="57"/>
       <c r="C80" s="33">
         <f>'Individual Treasure'!B10</f>
         <v>23.071499078512772</v>
       </c>
-      <c r="D80" s="48" t="s">
+      <c r="D80" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E80" s="49"/>
+      <c r="E80" s="47"/>
       <c r="F80" s="34">
         <f>SUMPRODUCT(C75:C79,F75:F79)</f>
         <v>23</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="50" t="s">
+      <c r="A81" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="B81" s="50"/>
-      <c r="C81" s="50"/>
-      <c r="D81" s="50"/>
-      <c r="E81" s="50"/>
-      <c r="F81" s="50"/>
-      <c r="G81" s="50"/>
-      <c r="H81" s="50"/>
-      <c r="I81" s="50"/>
-      <c r="J81" s="50"/>
-      <c r="K81" s="50"/>
-      <c r="L81" s="50"/>
+      <c r="B81" s="48"/>
+      <c r="C81" s="48"/>
+      <c r="D81" s="48"/>
+      <c r="E81" s="48"/>
+      <c r="F81" s="48"/>
+      <c r="G81" s="48"/>
+      <c r="H81" s="48"/>
+      <c r="I81" s="48"/>
+      <c r="J81" s="48"/>
+      <c r="K81" s="48"/>
+      <c r="L81" s="48"/>
     </row>
     <row r="82" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A82" s="51" t="s">
+      <c r="A82" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="B82" s="51"/>
-      <c r="C82" s="51"/>
-      <c r="D82" s="51"/>
-      <c r="E82" s="51"/>
-      <c r="F82" s="52"/>
+      <c r="B82" s="49"/>
+      <c r="C82" s="49"/>
+      <c r="D82" s="49"/>
+      <c r="E82" s="49"/>
+      <c r="F82" s="50"/>
     </row>
     <row r="83" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="53" t="s">
+      <c r="A83" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B83" s="54"/>
+      <c r="B83" s="52"/>
       <c r="C83" s="21">
         <v>5</v>
       </c>
-      <c r="D83" s="55" t="s">
+      <c r="D83" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E83" s="56"/>
-      <c r="F83" s="57"/>
+      <c r="E83" s="54"/>
+      <c r="F83" s="55"/>
     </row>
     <row r="84" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="42" t="s">
@@ -3731,82 +3752,82 @@
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A90" s="46" t="s">
+      <c r="A90" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B90" s="47"/>
+      <c r="B90" s="57"/>
       <c r="C90" s="33">
         <f>'Individual Treasure'!B11</f>
         <v>35.732264553480377</v>
       </c>
-      <c r="D90" s="48" t="s">
+      <c r="D90" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E90" s="49"/>
+      <c r="E90" s="47"/>
       <c r="F90" s="34">
         <f>SUMPRODUCT(C85:C89,F85:F89)</f>
         <v>35</v>
       </c>
     </row>
     <row r="91" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="50" t="s">
+      <c r="A91" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="B91" s="50"/>
-      <c r="C91" s="50"/>
-      <c r="D91" s="50"/>
-      <c r="E91" s="50"/>
-      <c r="F91" s="50"/>
-      <c r="G91" s="50"/>
-      <c r="H91" s="50"/>
-      <c r="I91" s="50"/>
-      <c r="J91" s="50"/>
-      <c r="K91" s="50"/>
-      <c r="L91" s="50"/>
+      <c r="B91" s="48"/>
+      <c r="C91" s="48"/>
+      <c r="D91" s="48"/>
+      <c r="E91" s="48"/>
+      <c r="F91" s="48"/>
+      <c r="G91" s="48"/>
+      <c r="H91" s="48"/>
+      <c r="I91" s="48"/>
+      <c r="J91" s="48"/>
+      <c r="K91" s="48"/>
+      <c r="L91" s="48"/>
     </row>
     <row r="92" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A92" s="51" t="s">
+      <c r="A92" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="B92" s="51"/>
-      <c r="C92" s="51"/>
-      <c r="D92" s="51"/>
-      <c r="E92" s="51"/>
-      <c r="F92" s="52"/>
-      <c r="G92" s="51" t="s">
+      <c r="B92" s="49"/>
+      <c r="C92" s="49"/>
+      <c r="D92" s="49"/>
+      <c r="E92" s="49"/>
+      <c r="F92" s="50"/>
+      <c r="G92" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="H92" s="51"/>
-      <c r="I92" s="51"/>
-      <c r="J92" s="51"/>
-      <c r="K92" s="51"/>
-      <c r="L92" s="52"/>
+      <c r="H92" s="49"/>
+      <c r="I92" s="49"/>
+      <c r="J92" s="49"/>
+      <c r="K92" s="49"/>
+      <c r="L92" s="50"/>
     </row>
     <row r="93" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="53" t="s">
+      <c r="A93" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B93" s="54"/>
+      <c r="B93" s="52"/>
       <c r="C93" s="21">
         <v>5</v>
       </c>
-      <c r="D93" s="55" t="s">
+      <c r="D93" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E93" s="56"/>
-      <c r="F93" s="57"/>
-      <c r="G93" s="53" t="s">
+      <c r="E93" s="54"/>
+      <c r="F93" s="55"/>
+      <c r="G93" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="H93" s="54"/>
+      <c r="H93" s="52"/>
       <c r="I93" s="21">
         <v>5</v>
       </c>
-      <c r="J93" s="55" t="s">
+      <c r="J93" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="K93" s="56"/>
-      <c r="L93" s="57"/>
+      <c r="K93" s="54"/>
+      <c r="L93" s="55"/>
     </row>
     <row r="94" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="42" t="s">
@@ -4069,78 +4090,78 @@
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A100" s="46" t="s">
+      <c r="A100" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B100" s="47"/>
+      <c r="B100" s="57"/>
       <c r="C100" s="33">
         <f>'Individual Treasure'!B12</f>
         <v>55.340778931397217</v>
       </c>
-      <c r="D100" s="48" t="s">
+      <c r="D100" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E100" s="49"/>
+      <c r="E100" s="47"/>
       <c r="F100" s="34">
         <f>SUMPRODUCT(C95:C99,F95:F99)</f>
         <v>55.25</v>
       </c>
-      <c r="G100" s="46" t="s">
+      <c r="G100" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="H100" s="47"/>
+      <c r="H100" s="57"/>
       <c r="I100" s="33">
         <f>'Individual Treasure'!B12</f>
         <v>55.340778931397217</v>
       </c>
-      <c r="J100" s="48" t="s">
+      <c r="J100" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="K100" s="49"/>
+      <c r="K100" s="47"/>
       <c r="L100" s="34">
         <f>SUMPRODUCT(I95:I99,L95:L99)</f>
         <v>56.25</v>
       </c>
     </row>
     <row r="101" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A101" s="50" t="s">
+      <c r="A101" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="B101" s="50"/>
-      <c r="C101" s="50"/>
-      <c r="D101" s="50"/>
-      <c r="E101" s="50"/>
-      <c r="F101" s="50"/>
-      <c r="G101" s="50"/>
-      <c r="H101" s="50"/>
-      <c r="I101" s="50"/>
-      <c r="J101" s="50"/>
-      <c r="K101" s="50"/>
-      <c r="L101" s="50"/>
+      <c r="B101" s="48"/>
+      <c r="C101" s="48"/>
+      <c r="D101" s="48"/>
+      <c r="E101" s="48"/>
+      <c r="F101" s="48"/>
+      <c r="G101" s="48"/>
+      <c r="H101" s="48"/>
+      <c r="I101" s="48"/>
+      <c r="J101" s="48"/>
+      <c r="K101" s="48"/>
+      <c r="L101" s="48"/>
     </row>
     <row r="102" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A102" s="51" t="s">
+      <c r="A102" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="B102" s="51"/>
-      <c r="C102" s="51"/>
-      <c r="D102" s="51"/>
-      <c r="E102" s="51"/>
-      <c r="F102" s="52"/>
+      <c r="B102" s="49"/>
+      <c r="C102" s="49"/>
+      <c r="D102" s="49"/>
+      <c r="E102" s="49"/>
+      <c r="F102" s="50"/>
     </row>
     <row r="103" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="53" t="s">
+      <c r="A103" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B103" s="54"/>
+      <c r="B103" s="52"/>
       <c r="C103" s="21">
         <v>5</v>
       </c>
-      <c r="D103" s="55" t="s">
+      <c r="D103" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E103" s="56"/>
-      <c r="F103" s="57"/>
+      <c r="E103" s="54"/>
+      <c r="F103" s="55"/>
     </row>
     <row r="104" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="42" t="s">
@@ -4279,62 +4300,62 @@
       </c>
     </row>
     <row r="110" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="46" t="s">
+      <c r="A110" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B110" s="47"/>
+      <c r="B110" s="57"/>
       <c r="C110" s="33">
         <f>'Individual Treasure'!B13</f>
         <v>85.709703849023938</v>
       </c>
-      <c r="D110" s="48" t="s">
+      <c r="D110" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E110" s="49"/>
+      <c r="E110" s="47"/>
       <c r="F110" s="34">
         <f>SUMPRODUCT(C105:C109,F105:F109)</f>
         <v>85.5</v>
       </c>
     </row>
     <row r="111" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A111" s="50" t="s">
+      <c r="A111" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="B111" s="50"/>
-      <c r="C111" s="50"/>
-      <c r="D111" s="50"/>
-      <c r="E111" s="50"/>
-      <c r="F111" s="50"/>
-      <c r="G111" s="50"/>
-      <c r="H111" s="50"/>
-      <c r="I111" s="50"/>
-      <c r="J111" s="50"/>
-      <c r="K111" s="50"/>
-      <c r="L111" s="50"/>
+      <c r="B111" s="48"/>
+      <c r="C111" s="48"/>
+      <c r="D111" s="48"/>
+      <c r="E111" s="48"/>
+      <c r="F111" s="48"/>
+      <c r="G111" s="48"/>
+      <c r="H111" s="48"/>
+      <c r="I111" s="48"/>
+      <c r="J111" s="48"/>
+      <c r="K111" s="48"/>
+      <c r="L111" s="48"/>
     </row>
     <row r="112" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A112" s="51" t="s">
+      <c r="A112" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="B112" s="51"/>
-      <c r="C112" s="51"/>
-      <c r="D112" s="51"/>
-      <c r="E112" s="51"/>
-      <c r="F112" s="52"/>
+      <c r="B112" s="49"/>
+      <c r="C112" s="49"/>
+      <c r="D112" s="49"/>
+      <c r="E112" s="49"/>
+      <c r="F112" s="50"/>
     </row>
     <row r="113" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="53" t="s">
+      <c r="A113" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B113" s="54"/>
+      <c r="B113" s="52"/>
       <c r="C113" s="21">
         <v>5</v>
       </c>
-      <c r="D113" s="55" t="s">
+      <c r="D113" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E113" s="56"/>
-      <c r="F113" s="57"/>
+      <c r="E113" s="54"/>
+      <c r="F113" s="55"/>
     </row>
     <row r="114" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="42" t="s">
@@ -4473,82 +4494,82 @@
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A120" s="46" t="s">
+      <c r="A120" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B120" s="47"/>
+      <c r="B120" s="57"/>
       <c r="C120" s="33">
         <f>'Individual Treasure'!B14</f>
         <v>132.7439453462336</v>
       </c>
-      <c r="D120" s="48" t="s">
+      <c r="D120" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E120" s="49"/>
+      <c r="E120" s="47"/>
       <c r="F120" s="34">
         <f>SUMPRODUCT(C115:C119,F115:F119)</f>
         <v>133</v>
       </c>
     </row>
     <row r="121" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A121" s="50" t="s">
+      <c r="A121" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="B121" s="50"/>
-      <c r="C121" s="50"/>
-      <c r="D121" s="50"/>
-      <c r="E121" s="50"/>
-      <c r="F121" s="50"/>
-      <c r="G121" s="50"/>
-      <c r="H121" s="50"/>
-      <c r="I121" s="50"/>
-      <c r="J121" s="50"/>
-      <c r="K121" s="50"/>
-      <c r="L121" s="50"/>
+      <c r="B121" s="48"/>
+      <c r="C121" s="48"/>
+      <c r="D121" s="48"/>
+      <c r="E121" s="48"/>
+      <c r="F121" s="48"/>
+      <c r="G121" s="48"/>
+      <c r="H121" s="48"/>
+      <c r="I121" s="48"/>
+      <c r="J121" s="48"/>
+      <c r="K121" s="48"/>
+      <c r="L121" s="48"/>
     </row>
     <row r="122" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A122" s="51" t="s">
+      <c r="A122" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B122" s="51"/>
-      <c r="C122" s="51"/>
-      <c r="D122" s="51"/>
-      <c r="E122" s="51"/>
-      <c r="F122" s="52"/>
-      <c r="G122" s="51" t="s">
+      <c r="B122" s="49"/>
+      <c r="C122" s="49"/>
+      <c r="D122" s="49"/>
+      <c r="E122" s="49"/>
+      <c r="F122" s="50"/>
+      <c r="G122" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="H122" s="51"/>
-      <c r="I122" s="51"/>
-      <c r="J122" s="51"/>
-      <c r="K122" s="51"/>
-      <c r="L122" s="52"/>
+      <c r="H122" s="49"/>
+      <c r="I122" s="49"/>
+      <c r="J122" s="49"/>
+      <c r="K122" s="49"/>
+      <c r="L122" s="50"/>
     </row>
     <row r="123" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="53" t="s">
+      <c r="A123" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B123" s="54"/>
+      <c r="B123" s="52"/>
       <c r="C123" s="21">
         <v>5</v>
       </c>
-      <c r="D123" s="55" t="s">
+      <c r="D123" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E123" s="56"/>
-      <c r="F123" s="57"/>
-      <c r="G123" s="53" t="s">
+      <c r="E123" s="54"/>
+      <c r="F123" s="55"/>
+      <c r="G123" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="H123" s="54"/>
+      <c r="H123" s="52"/>
       <c r="I123" s="21">
         <v>5</v>
       </c>
-      <c r="J123" s="55" t="s">
+      <c r="J123" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="K123" s="56"/>
-      <c r="L123" s="57"/>
+      <c r="K123" s="54"/>
+      <c r="L123" s="55"/>
     </row>
     <row r="124" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="42" t="s">
@@ -4811,78 +4832,78 @@
       </c>
     </row>
     <row r="130" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="46" t="s">
+      <c r="A130" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B130" s="47"/>
+      <c r="B130" s="57"/>
       <c r="C130" s="33">
         <f>'Individual Treasure'!B15</f>
         <v>205.58879840633722</v>
       </c>
-      <c r="D130" s="48" t="s">
+      <c r="D130" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E130" s="49"/>
+      <c r="E130" s="47"/>
       <c r="F130" s="34">
         <f>SUMPRODUCT(C125:C129,F125:F129)</f>
         <v>205</v>
       </c>
-      <c r="G130" s="46" t="s">
+      <c r="G130" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="H130" s="47"/>
+      <c r="H130" s="57"/>
       <c r="I130" s="33">
         <f>'Individual Treasure'!B15</f>
         <v>205.58879840633722</v>
       </c>
-      <c r="J130" s="48" t="s">
+      <c r="J130" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="K130" s="49"/>
+      <c r="K130" s="47"/>
       <c r="L130" s="34">
         <f>SUMPRODUCT(I125:I129,L125:L129)</f>
         <v>205.5</v>
       </c>
     </row>
     <row r="131" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A131" s="50" t="s">
+      <c r="A131" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="B131" s="50"/>
-      <c r="C131" s="50"/>
-      <c r="D131" s="50"/>
-      <c r="E131" s="50"/>
-      <c r="F131" s="50"/>
-      <c r="G131" s="50"/>
-      <c r="H131" s="50"/>
-      <c r="I131" s="50"/>
-      <c r="J131" s="50"/>
-      <c r="K131" s="50"/>
-      <c r="L131" s="50"/>
+      <c r="B131" s="48"/>
+      <c r="C131" s="48"/>
+      <c r="D131" s="48"/>
+      <c r="E131" s="48"/>
+      <c r="F131" s="48"/>
+      <c r="G131" s="48"/>
+      <c r="H131" s="48"/>
+      <c r="I131" s="48"/>
+      <c r="J131" s="48"/>
+      <c r="K131" s="48"/>
+      <c r="L131" s="48"/>
     </row>
     <row r="132" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A132" s="51" t="s">
+      <c r="A132" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="B132" s="51"/>
-      <c r="C132" s="51"/>
-      <c r="D132" s="51"/>
-      <c r="E132" s="51"/>
-      <c r="F132" s="52"/>
+      <c r="B132" s="49"/>
+      <c r="C132" s="49"/>
+      <c r="D132" s="49"/>
+      <c r="E132" s="49"/>
+      <c r="F132" s="50"/>
     </row>
     <row r="133" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A133" s="53" t="s">
+      <c r="A133" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B133" s="54"/>
+      <c r="B133" s="52"/>
       <c r="C133" s="21">
         <v>7</v>
       </c>
-      <c r="D133" s="55" t="s">
+      <c r="D133" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E133" s="56"/>
-      <c r="F133" s="57"/>
+      <c r="E133" s="54"/>
+      <c r="F133" s="55"/>
     </row>
     <row r="134" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="42" t="s">
@@ -5021,62 +5042,62 @@
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A140" s="46" t="s">
+      <c r="A140" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B140" s="47"/>
+      <c r="B140" s="57"/>
       <c r="C140" s="33">
         <f>'Individual Treasure'!B16</f>
         <v>318.40814976470659</v>
       </c>
-      <c r="D140" s="48" t="s">
+      <c r="D140" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E140" s="49"/>
+      <c r="E140" s="47"/>
       <c r="F140" s="34">
         <f>SUMPRODUCT(C135:C139,F135:F139)</f>
         <v>317.5</v>
       </c>
     </row>
     <row r="141" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A141" s="50" t="s">
+      <c r="A141" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="B141" s="50"/>
-      <c r="C141" s="50"/>
-      <c r="D141" s="50"/>
-      <c r="E141" s="50"/>
-      <c r="F141" s="50"/>
-      <c r="G141" s="50"/>
-      <c r="H141" s="50"/>
-      <c r="I141" s="50"/>
-      <c r="J141" s="50"/>
-      <c r="K141" s="50"/>
-      <c r="L141" s="50"/>
+      <c r="B141" s="48"/>
+      <c r="C141" s="48"/>
+      <c r="D141" s="48"/>
+      <c r="E141" s="48"/>
+      <c r="F141" s="48"/>
+      <c r="G141" s="48"/>
+      <c r="H141" s="48"/>
+      <c r="I141" s="48"/>
+      <c r="J141" s="48"/>
+      <c r="K141" s="48"/>
+      <c r="L141" s="48"/>
     </row>
     <row r="142" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A142" s="51" t="s">
+      <c r="A142" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="B142" s="51"/>
-      <c r="C142" s="51"/>
-      <c r="D142" s="51"/>
-      <c r="E142" s="51"/>
-      <c r="F142" s="52"/>
+      <c r="B142" s="49"/>
+      <c r="C142" s="49"/>
+      <c r="D142" s="49"/>
+      <c r="E142" s="49"/>
+      <c r="F142" s="50"/>
     </row>
     <row r="143" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="53" t="s">
+      <c r="A143" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B143" s="54"/>
+      <c r="B143" s="52"/>
       <c r="C143" s="21">
         <v>7</v>
       </c>
-      <c r="D143" s="55" t="s">
+      <c r="D143" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E143" s="56"/>
-      <c r="F143" s="57"/>
+      <c r="E143" s="54"/>
+      <c r="F143" s="55"/>
     </row>
     <row r="144" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="42" t="s">
@@ -5215,62 +5236,62 @@
       </c>
     </row>
     <row r="150" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="46" t="s">
+      <c r="A150" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B150" s="47"/>
+      <c r="B150" s="57"/>
       <c r="C150" s="33">
         <f>'Individual Treasure'!B17</f>
         <v>493.13849111663814</v>
       </c>
-      <c r="D150" s="48" t="s">
+      <c r="D150" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E150" s="49"/>
+      <c r="E150" s="47"/>
       <c r="F150" s="34">
         <f>SUMPRODUCT(C145:C149,F145:F149)</f>
         <v>495</v>
       </c>
     </row>
     <row r="151" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A151" s="50" t="s">
+      <c r="A151" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="B151" s="50"/>
-      <c r="C151" s="50"/>
-      <c r="D151" s="50"/>
-      <c r="E151" s="50"/>
-      <c r="F151" s="50"/>
-      <c r="G151" s="50"/>
-      <c r="H151" s="50"/>
-      <c r="I151" s="50"/>
-      <c r="J151" s="50"/>
-      <c r="K151" s="50"/>
-      <c r="L151" s="50"/>
+      <c r="B151" s="48"/>
+      <c r="C151" s="48"/>
+      <c r="D151" s="48"/>
+      <c r="E151" s="48"/>
+      <c r="F151" s="48"/>
+      <c r="G151" s="48"/>
+      <c r="H151" s="48"/>
+      <c r="I151" s="48"/>
+      <c r="J151" s="48"/>
+      <c r="K151" s="48"/>
+      <c r="L151" s="48"/>
     </row>
     <row r="152" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A152" s="51" t="s">
+      <c r="A152" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="B152" s="51"/>
-      <c r="C152" s="51"/>
-      <c r="D152" s="51"/>
-      <c r="E152" s="51"/>
-      <c r="F152" s="52"/>
+      <c r="B152" s="49"/>
+      <c r="C152" s="49"/>
+      <c r="D152" s="49"/>
+      <c r="E152" s="49"/>
+      <c r="F152" s="50"/>
     </row>
     <row r="153" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A153" s="53" t="s">
+      <c r="A153" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B153" s="54"/>
+      <c r="B153" s="52"/>
       <c r="C153" s="21">
         <v>7</v>
       </c>
-      <c r="D153" s="55" t="s">
+      <c r="D153" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E153" s="56"/>
-      <c r="F153" s="57"/>
+      <c r="E153" s="54"/>
+      <c r="F153" s="55"/>
     </row>
     <row r="154" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="42" t="s">
@@ -5409,62 +5430,62 @@
       </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A160" s="46" t="s">
+      <c r="A160" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B160" s="47"/>
+      <c r="B160" s="57"/>
       <c r="C160" s="33">
         <f>'Individual Treasure'!B18</f>
         <v>763.75423053869986</v>
       </c>
-      <c r="D160" s="48" t="s">
+      <c r="D160" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E160" s="49"/>
+      <c r="E160" s="47"/>
       <c r="F160" s="34">
         <f>SUMPRODUCT(C155:C159,F155:F159)</f>
         <v>760</v>
       </c>
     </row>
     <row r="161" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A161" s="50" t="s">
+      <c r="A161" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="B161" s="50"/>
-      <c r="C161" s="50"/>
-      <c r="D161" s="50"/>
-      <c r="E161" s="50"/>
-      <c r="F161" s="50"/>
-      <c r="G161" s="50"/>
-      <c r="H161" s="50"/>
-      <c r="I161" s="50"/>
-      <c r="J161" s="50"/>
-      <c r="K161" s="50"/>
-      <c r="L161" s="50"/>
+      <c r="B161" s="48"/>
+      <c r="C161" s="48"/>
+      <c r="D161" s="48"/>
+      <c r="E161" s="48"/>
+      <c r="F161" s="48"/>
+      <c r="G161" s="48"/>
+      <c r="H161" s="48"/>
+      <c r="I161" s="48"/>
+      <c r="J161" s="48"/>
+      <c r="K161" s="48"/>
+      <c r="L161" s="48"/>
     </row>
     <row r="162" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A162" s="51" t="s">
+      <c r="A162" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="B162" s="51"/>
-      <c r="C162" s="51"/>
-      <c r="D162" s="51"/>
-      <c r="E162" s="51"/>
-      <c r="F162" s="52"/>
+      <c r="B162" s="49"/>
+      <c r="C162" s="49"/>
+      <c r="D162" s="49"/>
+      <c r="E162" s="49"/>
+      <c r="F162" s="50"/>
     </row>
     <row r="163" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A163" s="53" t="s">
+      <c r="A163" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B163" s="54"/>
+      <c r="B163" s="52"/>
       <c r="C163" s="21">
         <v>7</v>
       </c>
-      <c r="D163" s="55" t="s">
+      <c r="D163" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E163" s="56"/>
-      <c r="F163" s="57"/>
+      <c r="E163" s="54"/>
+      <c r="F163" s="55"/>
     </row>
     <row r="164" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="42" t="s">
@@ -5603,82 +5624,82 @@
       </c>
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A170" s="46" t="s">
+      <c r="A170" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B170" s="47"/>
+      <c r="B170" s="57"/>
       <c r="C170" s="33">
         <f>'Individual Treasure'!B19</f>
         <v>1182.8736453829017</v>
       </c>
-      <c r="D170" s="48" t="s">
+      <c r="D170" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E170" s="49"/>
+      <c r="E170" s="47"/>
       <c r="F170" s="34">
         <f>SUMPRODUCT(C165:C169,F165:F169)</f>
         <v>1205.0000000000002</v>
       </c>
     </row>
     <row r="171" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A171" s="50" t="s">
+      <c r="A171" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="B171" s="50"/>
-      <c r="C171" s="50"/>
-      <c r="D171" s="50"/>
-      <c r="E171" s="50"/>
-      <c r="F171" s="50"/>
-      <c r="G171" s="50"/>
-      <c r="H171" s="50"/>
-      <c r="I171" s="50"/>
-      <c r="J171" s="50"/>
-      <c r="K171" s="50"/>
-      <c r="L171" s="50"/>
+      <c r="B171" s="48"/>
+      <c r="C171" s="48"/>
+      <c r="D171" s="48"/>
+      <c r="E171" s="48"/>
+      <c r="F171" s="48"/>
+      <c r="G171" s="48"/>
+      <c r="H171" s="48"/>
+      <c r="I171" s="48"/>
+      <c r="J171" s="48"/>
+      <c r="K171" s="48"/>
+      <c r="L171" s="48"/>
     </row>
     <row r="172" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A172" s="51" t="s">
+      <c r="A172" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="B172" s="51"/>
-      <c r="C172" s="51"/>
-      <c r="D172" s="51"/>
-      <c r="E172" s="51"/>
-      <c r="F172" s="52"/>
-      <c r="G172" s="66" t="s">
+      <c r="B172" s="49"/>
+      <c r="C172" s="49"/>
+      <c r="D172" s="49"/>
+      <c r="E172" s="49"/>
+      <c r="F172" s="50"/>
+      <c r="G172" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="H172" s="51"/>
-      <c r="I172" s="51"/>
-      <c r="J172" s="51"/>
-      <c r="K172" s="51"/>
-      <c r="L172" s="52"/>
+      <c r="H172" s="49"/>
+      <c r="I172" s="49"/>
+      <c r="J172" s="49"/>
+      <c r="K172" s="49"/>
+      <c r="L172" s="50"/>
     </row>
     <row r="173" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="53" t="s">
+      <c r="A173" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B173" s="54"/>
+      <c r="B173" s="52"/>
       <c r="C173" s="21">
         <v>7</v>
       </c>
-      <c r="D173" s="55" t="s">
+      <c r="D173" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E173" s="56"/>
-      <c r="F173" s="57"/>
-      <c r="G173" s="53" t="s">
+      <c r="E173" s="54"/>
+      <c r="F173" s="55"/>
+      <c r="G173" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="H173" s="54"/>
+      <c r="H173" s="52"/>
       <c r="I173" s="21">
         <v>7</v>
       </c>
-      <c r="J173" s="55" t="s">
+      <c r="J173" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="K173" s="56"/>
-      <c r="L173" s="57"/>
+      <c r="K173" s="54"/>
+      <c r="L173" s="55"/>
     </row>
     <row r="174" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A174" s="42" t="s">
@@ -5941,78 +5962,78 @@
       </c>
     </row>
     <row r="180" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="46" t="s">
+      <c r="A180" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B180" s="47"/>
+      <c r="B180" s="57"/>
       <c r="C180" s="33">
         <f>'Individual Treasure'!B20</f>
         <v>1831.989932094441</v>
       </c>
-      <c r="D180" s="48" t="s">
+      <c r="D180" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E180" s="49"/>
+      <c r="E180" s="47"/>
       <c r="F180" s="34">
         <f>SUMPRODUCT(C175:C179,F175:F179)</f>
         <v>1850.0000000000005</v>
       </c>
-      <c r="G180" s="46" t="s">
+      <c r="G180" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="H180" s="47"/>
+      <c r="H180" s="57"/>
       <c r="I180" s="33">
         <f>'Individual Treasure'!H20</f>
         <v>0</v>
       </c>
-      <c r="J180" s="48" t="s">
+      <c r="J180" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="K180" s="49"/>
+      <c r="K180" s="47"/>
       <c r="L180" s="34">
         <f>SUMPRODUCT(I175:I179,L175:L179)</f>
         <v>1850.0000000000005</v>
       </c>
     </row>
     <row r="181" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A181" s="50" t="s">
+      <c r="A181" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="B181" s="50"/>
-      <c r="C181" s="50"/>
-      <c r="D181" s="50"/>
-      <c r="E181" s="50"/>
-      <c r="F181" s="50"/>
-      <c r="G181" s="50"/>
-      <c r="H181" s="50"/>
-      <c r="I181" s="50"/>
-      <c r="J181" s="50"/>
-      <c r="K181" s="50"/>
-      <c r="L181" s="50"/>
+      <c r="B181" s="48"/>
+      <c r="C181" s="48"/>
+      <c r="D181" s="48"/>
+      <c r="E181" s="48"/>
+      <c r="F181" s="48"/>
+      <c r="G181" s="48"/>
+      <c r="H181" s="48"/>
+      <c r="I181" s="48"/>
+      <c r="J181" s="48"/>
+      <c r="K181" s="48"/>
+      <c r="L181" s="48"/>
     </row>
     <row r="182" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A182" s="51" t="s">
+      <c r="A182" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="B182" s="51"/>
-      <c r="C182" s="51"/>
-      <c r="D182" s="51"/>
-      <c r="E182" s="51"/>
-      <c r="F182" s="52"/>
+      <c r="B182" s="49"/>
+      <c r="C182" s="49"/>
+      <c r="D182" s="49"/>
+      <c r="E182" s="49"/>
+      <c r="F182" s="50"/>
     </row>
     <row r="183" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A183" s="53" t="s">
+      <c r="A183" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B183" s="54"/>
+      <c r="B183" s="52"/>
       <c r="C183" s="21">
         <v>7</v>
       </c>
-      <c r="D183" s="55" t="s">
+      <c r="D183" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="E183" s="56"/>
-      <c r="F183" s="57"/>
+      <c r="E183" s="54"/>
+      <c r="F183" s="55"/>
     </row>
     <row r="184" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="42" t="s">
@@ -6151,136 +6172,825 @@
       </c>
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A190" s="46" t="s">
+      <c r="A190" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B190" s="47"/>
+      <c r="B190" s="57"/>
       <c r="C190" s="33">
         <f>'Individual Treasure'!B21</f>
         <v>2837.3166689405625</v>
       </c>
-      <c r="D190" s="48" t="s">
+      <c r="D190" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E190" s="49"/>
+      <c r="E190" s="47"/>
       <c r="F190" s="34">
         <f>SUMPRODUCT(C185:C189,F185:F189)</f>
         <v>2850</v>
       </c>
     </row>
+    <row r="191" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A191" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="B191" s="48"/>
+      <c r="C191" s="48"/>
+      <c r="D191" s="48"/>
+      <c r="E191" s="48"/>
+      <c r="F191" s="48"/>
+      <c r="G191" s="48"/>
+      <c r="H191" s="48"/>
+      <c r="I191" s="48"/>
+      <c r="J191" s="48"/>
+      <c r="K191" s="48"/>
+      <c r="L191" s="48"/>
+    </row>
+    <row r="192" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A192" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="B192" s="49"/>
+      <c r="C192" s="49"/>
+      <c r="D192" s="49"/>
+      <c r="E192" s="49"/>
+      <c r="F192" s="50"/>
+    </row>
+    <row r="193" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A193" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B193" s="52"/>
+      <c r="C193" s="21">
+        <v>7</v>
+      </c>
+      <c r="D193" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="E193" s="54"/>
+      <c r="F193" s="55"/>
+    </row>
+    <row r="194" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A194" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B194" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C194" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D194" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E194" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F194" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A195" s="43">
+        <f>C193+1</f>
+        <v>8</v>
+      </c>
+      <c r="B195" s="8">
+        <v>9</v>
+      </c>
+      <c r="C195" s="31">
+        <f>((B195-A195+1)*0.05)</f>
+        <v>0.1</v>
+      </c>
+      <c r="D195" s="18">
+        <v>1</v>
+      </c>
+      <c r="E195" s="8">
+        <v>500</v>
+      </c>
+      <c r="F195" s="19">
+        <f>D195*E195</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A196" s="43">
+        <f>B195+1</f>
+        <v>10</v>
+      </c>
+      <c r="B196" s="8">
+        <v>11</v>
+      </c>
+      <c r="C196" s="31">
+        <f t="shared" ref="C196:C199" si="69">((B196-A196+1)*0.05)</f>
+        <v>0.1</v>
+      </c>
+      <c r="D196" s="18">
+        <v>3</v>
+      </c>
+      <c r="E196" s="8">
+        <v>500</v>
+      </c>
+      <c r="F196" s="19">
+        <f t="shared" ref="F196:F199" si="70">D196*E196</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A197" s="43">
+        <f t="shared" ref="A197:A199" si="71">B196+1</f>
+        <v>12</v>
+      </c>
+      <c r="B197" s="8">
+        <v>17</v>
+      </c>
+      <c r="C197" s="31">
+        <f t="shared" si="69"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="D197" s="18">
+        <v>2</v>
+      </c>
+      <c r="E197" s="8">
+        <v>1000</v>
+      </c>
+      <c r="F197" s="19">
+        <f t="shared" si="70"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A198" s="43">
+        <f t="shared" si="71"/>
+        <v>18</v>
+      </c>
+      <c r="B198" s="8">
+        <v>22</v>
+      </c>
+      <c r="C198" s="31">
+        <f t="shared" si="69"/>
+        <v>0.25</v>
+      </c>
+      <c r="D198" s="18">
+        <v>2</v>
+      </c>
+      <c r="E198" s="8">
+        <v>2000</v>
+      </c>
+      <c r="F198" s="19">
+        <f t="shared" si="70"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A199" s="43">
+        <f t="shared" si="71"/>
+        <v>23</v>
+      </c>
+      <c r="B199" s="44">
+        <f>20+C193</f>
+        <v>27</v>
+      </c>
+      <c r="C199" s="31">
+        <f t="shared" si="69"/>
+        <v>0.25</v>
+      </c>
+      <c r="D199" s="20">
+        <v>1</v>
+      </c>
+      <c r="E199" s="28">
+        <v>10000</v>
+      </c>
+      <c r="F199" s="22">
+        <f t="shared" si="70"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A200" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B200" s="57"/>
+      <c r="C200" s="33">
+        <f>'Individual Treasure'!B22</f>
+        <v>4394.3286689596089</v>
+      </c>
+      <c r="D200" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="E200" s="47"/>
+      <c r="F200" s="34">
+        <f>SUMPRODUCT(C195:C199,F195:F199)</f>
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A201" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="B201" s="48"/>
+      <c r="C201" s="48"/>
+      <c r="D201" s="48"/>
+      <c r="E201" s="48"/>
+      <c r="F201" s="48"/>
+      <c r="G201" s="48"/>
+      <c r="H201" s="48"/>
+      <c r="I201" s="48"/>
+      <c r="J201" s="48"/>
+      <c r="K201" s="48"/>
+      <c r="L201" s="48"/>
+    </row>
+    <row r="202" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A202" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B202" s="49"/>
+      <c r="C202" s="49"/>
+      <c r="D202" s="49"/>
+      <c r="E202" s="49"/>
+      <c r="F202" s="50"/>
+    </row>
+    <row r="203" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A203" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B203" s="52"/>
+      <c r="C203" s="21">
+        <v>7</v>
+      </c>
+      <c r="D203" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="E203" s="54"/>
+      <c r="F203" s="55"/>
+    </row>
+    <row r="204" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A204" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B204" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C204" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D204" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E204" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F204" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A205" s="43">
+        <f>C203+1</f>
+        <v>8</v>
+      </c>
+      <c r="B205" s="8">
+        <v>9</v>
+      </c>
+      <c r="C205" s="31">
+        <f>((B205-A205+1)*0.05)</f>
+        <v>0.1</v>
+      </c>
+      <c r="D205" s="18">
+        <v>2</v>
+      </c>
+      <c r="E205" s="8">
+        <v>500</v>
+      </c>
+      <c r="F205" s="19">
+        <f>D205*E205</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A206" s="43">
+        <f>B205+1</f>
+        <v>10</v>
+      </c>
+      <c r="B206" s="8">
+        <v>11</v>
+      </c>
+      <c r="C206" s="31">
+        <f t="shared" ref="C206:C209" si="72">((B206-A206+1)*0.05)</f>
+        <v>0.1</v>
+      </c>
+      <c r="D206" s="18">
+        <v>3</v>
+      </c>
+      <c r="E206" s="8">
+        <v>1000</v>
+      </c>
+      <c r="F206" s="19">
+        <f t="shared" ref="F206:F209" si="73">D206*E206</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A207" s="43">
+        <f t="shared" ref="A207:A209" si="74">B206+1</f>
+        <v>12</v>
+      </c>
+      <c r="B207" s="8">
+        <v>18</v>
+      </c>
+      <c r="C207" s="31">
+        <f t="shared" si="72"/>
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="D207" s="18">
+        <v>1</v>
+      </c>
+      <c r="E207" s="8">
+        <v>10000</v>
+      </c>
+      <c r="F207" s="19">
+        <f t="shared" si="73"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A208" s="43">
+        <f t="shared" si="74"/>
+        <v>19</v>
+      </c>
+      <c r="B208" s="8">
+        <v>23</v>
+      </c>
+      <c r="C208" s="31">
+        <f t="shared" si="72"/>
+        <v>0.25</v>
+      </c>
+      <c r="D208" s="18">
+        <v>2</v>
+      </c>
+      <c r="E208" s="8">
+        <v>10000</v>
+      </c>
+      <c r="F208" s="19">
+        <f t="shared" si="73"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A209" s="43">
+        <f t="shared" si="74"/>
+        <v>24</v>
+      </c>
+      <c r="B209" s="44">
+        <f>20+C203</f>
+        <v>27</v>
+      </c>
+      <c r="C209" s="31">
+        <f t="shared" si="72"/>
+        <v>0.2</v>
+      </c>
+      <c r="D209" s="20">
+        <v>2</v>
+      </c>
+      <c r="E209" s="28">
+        <v>20000</v>
+      </c>
+      <c r="F209" s="22">
+        <f t="shared" si="73"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A210" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B210" s="57"/>
+      <c r="C210" s="33">
+        <f>'Individual Treasure'!B25</f>
+        <v>16324.756685731661</v>
+      </c>
+      <c r="D210" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="E210" s="47"/>
+      <c r="F210" s="34">
+        <f>SUMPRODUCT(C205:C209,F205:F209)</f>
+        <v>16900</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A211" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="B211" s="48"/>
+      <c r="C211" s="48"/>
+      <c r="D211" s="48"/>
+      <c r="E211" s="48"/>
+      <c r="F211" s="48"/>
+      <c r="G211" s="48"/>
+      <c r="H211" s="48"/>
+      <c r="I211" s="48"/>
+      <c r="J211" s="48"/>
+      <c r="K211" s="48"/>
+      <c r="L211" s="48"/>
+    </row>
+    <row r="212" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A212" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B212" s="49"/>
+      <c r="C212" s="49"/>
+      <c r="D212" s="49"/>
+      <c r="E212" s="49"/>
+      <c r="F212" s="50"/>
+    </row>
+    <row r="213" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A213" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B213" s="52"/>
+      <c r="C213" s="21">
+        <v>7</v>
+      </c>
+      <c r="D213" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="E213" s="54"/>
+      <c r="F213" s="55"/>
+    </row>
+    <row r="214" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A214" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B214" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C214" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D214" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E214" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F214" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A215" s="43">
+        <f>C213+1</f>
+        <v>8</v>
+      </c>
+      <c r="B215" s="8">
+        <v>9</v>
+      </c>
+      <c r="C215" s="31">
+        <f>((B215-A215+1)*0.05)</f>
+        <v>0.1</v>
+      </c>
+      <c r="D215" s="18">
+        <v>2</v>
+      </c>
+      <c r="E215" s="8">
+        <v>5000</v>
+      </c>
+      <c r="F215" s="19">
+        <f>D215*E215</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A216" s="43">
+        <f>B215+1</f>
+        <v>10</v>
+      </c>
+      <c r="B216" s="8">
+        <v>13</v>
+      </c>
+      <c r="C216" s="31">
+        <f t="shared" ref="C216:C219" si="75">((B216-A216+1)*0.05)</f>
+        <v>0.2</v>
+      </c>
+      <c r="D216" s="18">
+        <v>3</v>
+      </c>
+      <c r="E216" s="8">
+        <v>10000</v>
+      </c>
+      <c r="F216" s="19">
+        <f t="shared" ref="F216:F219" si="76">D216*E216</f>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A217" s="43">
+        <f t="shared" ref="A217:A219" si="77">B216+1</f>
+        <v>14</v>
+      </c>
+      <c r="B217" s="8">
+        <v>18</v>
+      </c>
+      <c r="C217" s="31">
+        <f t="shared" si="75"/>
+        <v>0.25</v>
+      </c>
+      <c r="D217" s="18">
+        <v>2</v>
+      </c>
+      <c r="E217" s="8">
+        <v>20000</v>
+      </c>
+      <c r="F217" s="19">
+        <f t="shared" si="76"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A218" s="43">
+        <f t="shared" si="77"/>
+        <v>19</v>
+      </c>
+      <c r="B218" s="8">
+        <v>23</v>
+      </c>
+      <c r="C218" s="31">
+        <f t="shared" si="75"/>
+        <v>0.25</v>
+      </c>
+      <c r="D218" s="18">
+        <v>2</v>
+      </c>
+      <c r="E218" s="8">
+        <v>20000</v>
+      </c>
+      <c r="F218" s="19">
+        <f t="shared" si="76"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A219" s="43">
+        <f t="shared" si="77"/>
+        <v>24</v>
+      </c>
+      <c r="B219" s="44">
+        <f>20+C213</f>
+        <v>27</v>
+      </c>
+      <c r="C219" s="31">
+        <f t="shared" si="75"/>
+        <v>0.2</v>
+      </c>
+      <c r="D219" s="20">
+        <v>3</v>
+      </c>
+      <c r="E219" s="28">
+        <v>20000</v>
+      </c>
+      <c r="F219" s="22">
+        <f t="shared" si="76"/>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A220" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B220" s="57"/>
+      <c r="C220" s="33">
+        <f>'Individual Treasure'!B27</f>
+        <v>39157.609472169628</v>
+      </c>
+      <c r="D220" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="E220" s="47"/>
+      <c r="F220" s="34">
+        <f>SUMPRODUCT(C215:C219,F215:F219)</f>
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="221" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A221" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B221" s="48"/>
+      <c r="C221" s="48"/>
+      <c r="D221" s="48"/>
+      <c r="E221" s="48"/>
+      <c r="F221" s="48"/>
+      <c r="G221" s="48"/>
+      <c r="H221" s="48"/>
+      <c r="I221" s="48"/>
+      <c r="J221" s="48"/>
+      <c r="K221" s="48"/>
+      <c r="L221" s="48"/>
+    </row>
+    <row r="222" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A222" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B222" s="49"/>
+      <c r="C222" s="49"/>
+      <c r="D222" s="49"/>
+      <c r="E222" s="49"/>
+      <c r="F222" s="50"/>
+    </row>
+    <row r="223" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A223" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B223" s="52"/>
+      <c r="C223" s="21">
+        <v>7</v>
+      </c>
+      <c r="D223" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="E223" s="54"/>
+      <c r="F223" s="55"/>
+    </row>
+    <row r="224" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A224" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B224" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C224" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D224" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E224" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F224" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" s="43">
+        <f>C223+1</f>
+        <v>8</v>
+      </c>
+      <c r="B225" s="8">
+        <v>9</v>
+      </c>
+      <c r="C225" s="31">
+        <f>((B225-A225+1)*0.05)</f>
+        <v>0.1</v>
+      </c>
+      <c r="D225" s="18">
+        <v>2</v>
+      </c>
+      <c r="E225" s="8">
+        <v>20000</v>
+      </c>
+      <c r="F225" s="19">
+        <f>D225*E225</f>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226" s="43">
+        <f>B225+1</f>
+        <v>10</v>
+      </c>
+      <c r="B226" s="8">
+        <v>14</v>
+      </c>
+      <c r="C226" s="31">
+        <f t="shared" ref="C226:C229" si="78">((B226-A226+1)*0.05)</f>
+        <v>0.25</v>
+      </c>
+      <c r="D226" s="18">
+        <v>3</v>
+      </c>
+      <c r="E226" s="8">
+        <v>20000</v>
+      </c>
+      <c r="F226" s="19">
+        <f t="shared" ref="F226:F229" si="79">D226*E226</f>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" s="43">
+        <f t="shared" ref="A227:A229" si="80">B226+1</f>
+        <v>15</v>
+      </c>
+      <c r="B227" s="8">
+        <v>18</v>
+      </c>
+      <c r="C227" s="31">
+        <f t="shared" si="78"/>
+        <v>0.2</v>
+      </c>
+      <c r="D227" s="18">
+        <v>1</v>
+      </c>
+      <c r="E227" s="8">
+        <v>100000</v>
+      </c>
+      <c r="F227" s="19">
+        <f t="shared" si="79"/>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" s="43">
+        <f t="shared" si="80"/>
+        <v>19</v>
+      </c>
+      <c r="B228" s="8">
+        <v>25</v>
+      </c>
+      <c r="C228" s="31">
+        <f t="shared" si="78"/>
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="D228" s="18">
+        <v>1</v>
+      </c>
+      <c r="E228" s="8">
+        <v>100000</v>
+      </c>
+      <c r="F228" s="19">
+        <f t="shared" si="79"/>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" s="43">
+        <f t="shared" si="80"/>
+        <v>26</v>
+      </c>
+      <c r="B229" s="44">
+        <f>20+C223</f>
+        <v>27</v>
+      </c>
+      <c r="C229" s="31">
+        <f t="shared" si="78"/>
+        <v>0.1</v>
+      </c>
+      <c r="D229" s="20">
+        <v>2</v>
+      </c>
+      <c r="E229" s="28">
+        <v>100000</v>
+      </c>
+      <c r="F229" s="22">
+        <f t="shared" si="79"/>
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B230" s="57"/>
+      <c r="C230" s="33">
+        <f>'Individual Treasure'!B29</f>
+        <v>93925.956085772239</v>
+      </c>
+      <c r="D230" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="E230" s="47"/>
+      <c r="F230" s="34">
+        <f>SUMPRODUCT(C225:C229,F225:F229)</f>
+        <v>94000</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="134">
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="A31:L31"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="G92:L92"/>
-    <mergeCell ref="G93:H93"/>
-    <mergeCell ref="J93:L93"/>
-    <mergeCell ref="G100:H100"/>
-    <mergeCell ref="J100:K100"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G22:L22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="A51:L51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="A41:L41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="A71:L71"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="A61:L61"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="A91:L91"/>
-    <mergeCell ref="A92:F92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:F93"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="A81:L81"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="A111:L111"/>
-    <mergeCell ref="A112:F112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="D113:F113"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="D120:E120"/>
-    <mergeCell ref="A101:L101"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="D103:F103"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="A131:L131"/>
-    <mergeCell ref="A132:F132"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="D133:F133"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="D140:E140"/>
-    <mergeCell ref="A121:L121"/>
-    <mergeCell ref="A122:F122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="D123:F123"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="G122:L122"/>
-    <mergeCell ref="G123:H123"/>
-    <mergeCell ref="J123:L123"/>
-    <mergeCell ref="G130:H130"/>
-    <mergeCell ref="J130:K130"/>
-    <mergeCell ref="A151:L151"/>
-    <mergeCell ref="A152:F152"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="D153:F153"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="D160:E160"/>
-    <mergeCell ref="A141:L141"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="D143:F143"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="D150:E150"/>
+  <mergeCells count="158">
+    <mergeCell ref="A222:F222"/>
+    <mergeCell ref="A223:B223"/>
+    <mergeCell ref="D223:F223"/>
+    <mergeCell ref="A230:B230"/>
+    <mergeCell ref="D230:E230"/>
+    <mergeCell ref="A210:B210"/>
+    <mergeCell ref="D210:E210"/>
+    <mergeCell ref="A211:L211"/>
+    <mergeCell ref="A212:F212"/>
+    <mergeCell ref="A213:B213"/>
+    <mergeCell ref="D213:F213"/>
+    <mergeCell ref="A220:B220"/>
+    <mergeCell ref="D220:E220"/>
+    <mergeCell ref="A221:L221"/>
+    <mergeCell ref="A191:L191"/>
+    <mergeCell ref="A192:F192"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="D193:F193"/>
+    <mergeCell ref="A200:B200"/>
+    <mergeCell ref="D200:E200"/>
+    <mergeCell ref="A201:L201"/>
+    <mergeCell ref="A202:F202"/>
+    <mergeCell ref="A203:B203"/>
+    <mergeCell ref="D203:F203"/>
     <mergeCell ref="A180:B180"/>
     <mergeCell ref="D180:E180"/>
     <mergeCell ref="A181:L181"/>
@@ -6304,6 +7014,117 @@
     <mergeCell ref="J173:L173"/>
     <mergeCell ref="G180:H180"/>
     <mergeCell ref="J180:K180"/>
+    <mergeCell ref="A151:L151"/>
+    <mergeCell ref="A152:F152"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="D153:F153"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="D160:E160"/>
+    <mergeCell ref="A141:L141"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="D143:F143"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="A131:L131"/>
+    <mergeCell ref="A132:F132"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="D133:F133"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="D140:E140"/>
+    <mergeCell ref="A121:L121"/>
+    <mergeCell ref="A122:F122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="D123:F123"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="G122:L122"/>
+    <mergeCell ref="G123:H123"/>
+    <mergeCell ref="J123:L123"/>
+    <mergeCell ref="G130:H130"/>
+    <mergeCell ref="J130:K130"/>
+    <mergeCell ref="A111:L111"/>
+    <mergeCell ref="A112:F112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D113:F113"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="A101:L101"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="D103:F103"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="A91:L91"/>
+    <mergeCell ref="A92:F92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:F93"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="A81:L81"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="A71:L71"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="A61:L61"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G22:L22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="A31:L31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="G92:L92"/>
+    <mergeCell ref="G93:H93"/>
+    <mergeCell ref="J93:L93"/>
+    <mergeCell ref="G100:H100"/>
+    <mergeCell ref="J100:K100"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="A51:L51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A41:L41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6347,37 +7168,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="63"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="64"/>
     </row>
     <row r="2" spans="1:23" s="14" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
       <c r="C2" s="60" t="s">
         <v>12</v>
       </c>
@@ -6982,37 +7803,37 @@
       <c r="W10" s="12"/>
     </row>
     <row r="11" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="63"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="63"/>
-      <c r="N11" s="63"/>
-      <c r="O11" s="63"/>
-      <c r="P11" s="63"/>
-      <c r="Q11" s="63"/>
-      <c r="R11" s="63"/>
-      <c r="S11" s="63"/>
-      <c r="T11" s="63"/>
-      <c r="U11" s="63"/>
-      <c r="V11" s="63"/>
-      <c r="W11" s="63"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="64"/>
+      <c r="P11" s="64"/>
+      <c r="Q11" s="64"/>
+      <c r="R11" s="64"/>
+      <c r="S11" s="64"/>
+      <c r="T11" s="64"/>
+      <c r="U11" s="64"/>
+      <c r="V11" s="64"/>
+      <c r="W11" s="64"/>
     </row>
     <row r="12" spans="1:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="65"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="60" t="s">
         <v>38</v>
       </c>
@@ -7266,37 +8087,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="63"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="64"/>
     </row>
     <row r="2" spans="1:23" s="14" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
       <c r="C2" s="60" t="s">
         <v>12</v>
       </c>
@@ -7901,37 +8722,37 @@
       <c r="W10" s="12"/>
     </row>
     <row r="11" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="63"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="63"/>
-      <c r="N11" s="63"/>
-      <c r="O11" s="63"/>
-      <c r="P11" s="63"/>
-      <c r="Q11" s="63"/>
-      <c r="R11" s="63"/>
-      <c r="S11" s="63"/>
-      <c r="T11" s="63"/>
-      <c r="U11" s="63"/>
-      <c r="V11" s="63"/>
-      <c r="W11" s="63"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="64"/>
+      <c r="P11" s="64"/>
+      <c r="Q11" s="64"/>
+      <c r="R11" s="64"/>
+      <c r="S11" s="64"/>
+      <c r="T11" s="64"/>
+      <c r="U11" s="64"/>
+      <c r="V11" s="64"/>
+      <c r="W11" s="64"/>
     </row>
     <row r="12" spans="1:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="65"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="60" t="s">
         <v>38</v>
       </c>
@@ -8185,37 +9006,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="63"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="64"/>
     </row>
     <row r="2" spans="1:23" s="14" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="65"/>
       <c r="C2" s="60" t="s">
         <v>12</v>
       </c>
@@ -8820,37 +9641,37 @@
       <c r="W10" s="12"/>
     </row>
     <row r="11" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="63"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="63"/>
-      <c r="N11" s="63"/>
-      <c r="O11" s="63"/>
-      <c r="P11" s="63"/>
-      <c r="Q11" s="63"/>
-      <c r="R11" s="63"/>
-      <c r="S11" s="63"/>
-      <c r="T11" s="63"/>
-      <c r="U11" s="63"/>
-      <c r="V11" s="63"/>
-      <c r="W11" s="63"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="64"/>
+      <c r="P11" s="64"/>
+      <c r="Q11" s="64"/>
+      <c r="R11" s="64"/>
+      <c r="S11" s="64"/>
+      <c r="T11" s="64"/>
+      <c r="U11" s="64"/>
+      <c r="V11" s="64"/>
+      <c r="W11" s="64"/>
     </row>
     <row r="12" spans="1:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="65"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="60" t="s">
         <v>38</v>
       </c>

</xml_diff>